<commit_message>
Added a SPARQL Optimisation which makes queries scale better as dataset size increases
</commit_message>
<xml_diff>
--- a/Benchmarks/dotNetRDF BSBM Benchmark.xlsx
+++ b/Benchmarks/dotNetRDF BSBM Benchmark.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="58">
   <si>
     <t>BSBM Benchmarks</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>Leviathan Engine - Version 0.4.1 using Statistics Optimiser with 4 Clients</t>
+  </si>
+  <si>
+    <t>Leviathan Engine - Version 0.4.2 using Default Optimiser</t>
   </si>
 </sst>
 </file>
@@ -477,8 +480,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -531,12 +540,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,7 +569,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1128,11 +1130,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="81384576"/>
-        <c:axId val="81386112"/>
+        <c:axId val="56537472"/>
+        <c:axId val="56539008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="81384576"/>
+        <c:axId val="56537472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1140,14 +1142,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81386112"/>
+        <c:crossAx val="56539008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81386112"/>
+        <c:axId val="56539008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1169,25 +1171,23 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81384576"/>
+        <c:crossAx val="56537472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1213,7 +1213,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1526,11 +1525,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="81419264"/>
-        <c:axId val="81429248"/>
+        <c:axId val="56871168"/>
+        <c:axId val="56881152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="81419264"/>
+        <c:axId val="56871168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1538,14 +1537,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81429248"/>
+        <c:crossAx val="56881152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81429248"/>
+        <c:axId val="56881152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1567,25 +1566,23 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81419264"/>
+        <c:crossAx val="56871168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1791,25 +1788,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="81446400"/>
-        <c:axId val="81447936"/>
+        <c:axId val="57168640"/>
+        <c:axId val="57170176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="81446400"/>
+        <c:axId val="57168640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81447936"/>
+        <c:crossAx val="57170176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81447936"/>
+        <c:axId val="57170176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1834,7 +1831,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81446400"/>
+        <c:crossAx val="57168640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1846,7 +1843,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1872,7 +1869,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2179,25 +2175,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="83519360"/>
-        <c:axId val="83520896"/>
+        <c:axId val="62686336"/>
+        <c:axId val="62687872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83519360"/>
+        <c:axId val="62686336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83520896"/>
+        <c:crossAx val="62687872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83520896"/>
+        <c:axId val="62687872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2219,24 +2215,22 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83519360"/>
+        <c:crossAx val="62686336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2657,11 +2651,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L116"/>
+  <dimension ref="A1:L126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G113" sqref="G113"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G121" sqref="G121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2680,34 +2674,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1">
       <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="15.75">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42" t="s">
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42" t="s">
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="6" t="s">
@@ -2748,20 +2742,20 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="41"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="43"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="5">
@@ -2840,20 +2834,20 @@
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="40"/>
-      <c r="L8" s="41"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="43"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="8">
@@ -3008,20 +3002,20 @@
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="40"/>
-      <c r="L13" s="41"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="43"/>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="5">
@@ -3252,20 +3246,20 @@
       </c>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="40"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="41"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="43"/>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="8">
@@ -3382,20 +3376,20 @@
       </c>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="39" t="s">
+      <c r="A24" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="41"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="43"/>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="8">
@@ -3626,20 +3620,20 @@
       </c>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="39" t="s">
+      <c r="A31" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
-      <c r="K31" s="40"/>
-      <c r="L31" s="41"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="42"/>
+      <c r="J31" s="42"/>
+      <c r="K31" s="42"/>
+      <c r="L31" s="43"/>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="8">
@@ -3794,20 +3788,20 @@
       </c>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="40"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="40"/>
-      <c r="F36" s="40"/>
-      <c r="G36" s="40"/>
-      <c r="H36" s="40"/>
-      <c r="I36" s="40"/>
-      <c r="J36" s="40"/>
-      <c r="K36" s="40"/>
-      <c r="L36" s="41"/>
+      <c r="B36" s="42"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="42"/>
+      <c r="G36" s="42"/>
+      <c r="H36" s="42"/>
+      <c r="I36" s="42"/>
+      <c r="J36" s="42"/>
+      <c r="K36" s="42"/>
+      <c r="L36" s="43"/>
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="8">
@@ -4114,20 +4108,20 @@
       </c>
     </row>
     <row r="45" spans="1:12">
-      <c r="A45" s="28" t="s">
+      <c r="A45" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="B45" s="28"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="28"/>
-      <c r="H45" s="28"/>
-      <c r="I45" s="28"/>
-      <c r="J45" s="28"/>
-      <c r="K45" s="28"/>
-      <c r="L45" s="28"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="29"/>
+      <c r="I45" s="29"/>
+      <c r="J45" s="29"/>
+      <c r="K45" s="29"/>
+      <c r="L45" s="29"/>
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="8">
@@ -4498,20 +4492,20 @@
       <c r="L55" s="8"/>
     </row>
     <row r="56" spans="1:12">
-      <c r="A56" s="43" t="s">
+      <c r="A56" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="B56" s="43"/>
-      <c r="C56" s="43"/>
-      <c r="D56" s="43"/>
-      <c r="E56" s="43"/>
-      <c r="F56" s="43"/>
-      <c r="G56" s="43"/>
-      <c r="H56" s="43"/>
-      <c r="I56" s="43"/>
-      <c r="J56" s="43"/>
-      <c r="K56" s="43"/>
-      <c r="L56" s="43"/>
+      <c r="B56" s="45"/>
+      <c r="C56" s="45"/>
+      <c r="D56" s="45"/>
+      <c r="E56" s="45"/>
+      <c r="F56" s="45"/>
+      <c r="G56" s="45"/>
+      <c r="H56" s="45"/>
+      <c r="I56" s="45"/>
+      <c r="J56" s="45"/>
+      <c r="K56" s="45"/>
+      <c r="L56" s="45"/>
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="19">
@@ -4532,14 +4526,14 @@
       <c r="F57" s="19">
         <v>50</v>
       </c>
-      <c r="G57" s="29" t="s">
+      <c r="G57" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="H57" s="30"/>
-      <c r="I57" s="30"/>
-      <c r="J57" s="30"/>
-      <c r="K57" s="30"/>
-      <c r="L57" s="31"/>
+      <c r="H57" s="32"/>
+      <c r="I57" s="32"/>
+      <c r="J57" s="32"/>
+      <c r="K57" s="32"/>
+      <c r="L57" s="33"/>
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="19">
@@ -4560,12 +4554,12 @@
       <c r="F58" s="19">
         <v>50</v>
       </c>
-      <c r="G58" s="32"/>
-      <c r="H58" s="33"/>
-      <c r="I58" s="33"/>
-      <c r="J58" s="33"/>
-      <c r="K58" s="33"/>
-      <c r="L58" s="34"/>
+      <c r="G58" s="34"/>
+      <c r="H58" s="35"/>
+      <c r="I58" s="35"/>
+      <c r="J58" s="35"/>
+      <c r="K58" s="35"/>
+      <c r="L58" s="36"/>
     </row>
     <row r="59" spans="1:12">
       <c r="A59" s="19">
@@ -4586,12 +4580,12 @@
       <c r="F59" s="19">
         <v>50</v>
       </c>
-      <c r="G59" s="32"/>
-      <c r="H59" s="33"/>
-      <c r="I59" s="33"/>
-      <c r="J59" s="33"/>
-      <c r="K59" s="33"/>
-      <c r="L59" s="34"/>
+      <c r="G59" s="34"/>
+      <c r="H59" s="35"/>
+      <c r="I59" s="35"/>
+      <c r="J59" s="35"/>
+      <c r="K59" s="35"/>
+      <c r="L59" s="36"/>
     </row>
     <row r="60" spans="1:12">
       <c r="A60" s="19">
@@ -4612,12 +4606,12 @@
       <c r="F60" s="19">
         <v>50</v>
       </c>
-      <c r="G60" s="32"/>
-      <c r="H60" s="33"/>
-      <c r="I60" s="33"/>
-      <c r="J60" s="33"/>
-      <c r="K60" s="33"/>
-      <c r="L60" s="34"/>
+      <c r="G60" s="34"/>
+      <c r="H60" s="35"/>
+      <c r="I60" s="35"/>
+      <c r="J60" s="35"/>
+      <c r="K60" s="35"/>
+      <c r="L60" s="36"/>
     </row>
     <row r="61" spans="1:12">
       <c r="A61" s="19">
@@ -4638,12 +4632,12 @@
       <c r="F61" s="19">
         <v>50</v>
       </c>
-      <c r="G61" s="32"/>
-      <c r="H61" s="33"/>
-      <c r="I61" s="33"/>
-      <c r="J61" s="33"/>
-      <c r="K61" s="33"/>
-      <c r="L61" s="34"/>
+      <c r="G61" s="34"/>
+      <c r="H61" s="35"/>
+      <c r="I61" s="35"/>
+      <c r="J61" s="35"/>
+      <c r="K61" s="35"/>
+      <c r="L61" s="36"/>
     </row>
     <row r="62" spans="1:12">
       <c r="A62" s="19">
@@ -4664,12 +4658,12 @@
       <c r="F62" s="19">
         <v>50</v>
       </c>
-      <c r="G62" s="32"/>
-      <c r="H62" s="33"/>
-      <c r="I62" s="33"/>
-      <c r="J62" s="33"/>
-      <c r="K62" s="33"/>
-      <c r="L62" s="34"/>
+      <c r="G62" s="34"/>
+      <c r="H62" s="35"/>
+      <c r="I62" s="35"/>
+      <c r="J62" s="35"/>
+      <c r="K62" s="35"/>
+      <c r="L62" s="36"/>
     </row>
     <row r="63" spans="1:12">
       <c r="A63" s="22">
@@ -4690,12 +4684,12 @@
       <c r="F63" s="19">
         <v>50</v>
       </c>
-      <c r="G63" s="32"/>
-      <c r="H63" s="33"/>
-      <c r="I63" s="33"/>
-      <c r="J63" s="33"/>
-      <c r="K63" s="33"/>
-      <c r="L63" s="34"/>
+      <c r="G63" s="34"/>
+      <c r="H63" s="35"/>
+      <c r="I63" s="35"/>
+      <c r="J63" s="35"/>
+      <c r="K63" s="35"/>
+      <c r="L63" s="36"/>
     </row>
     <row r="64" spans="1:12">
       <c r="A64" s="22">
@@ -4716,12 +4710,12 @@
       <c r="F64" s="19">
         <v>50</v>
       </c>
-      <c r="G64" s="35"/>
-      <c r="H64" s="36"/>
-      <c r="I64" s="36"/>
-      <c r="J64" s="36"/>
-      <c r="K64" s="36"/>
-      <c r="L64" s="37"/>
+      <c r="G64" s="37"/>
+      <c r="H64" s="38"/>
+      <c r="I64" s="38"/>
+      <c r="J64" s="38"/>
+      <c r="K64" s="38"/>
+      <c r="L64" s="39"/>
     </row>
     <row r="65" spans="1:12">
       <c r="A65" s="22">
@@ -4762,20 +4756,20 @@
       </c>
     </row>
     <row r="66" spans="1:12">
-      <c r="A66" s="28" t="s">
+      <c r="A66" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="B66" s="28"/>
-      <c r="C66" s="28"/>
-      <c r="D66" s="28"/>
-      <c r="E66" s="28"/>
-      <c r="F66" s="28"/>
-      <c r="G66" s="28"/>
-      <c r="H66" s="28"/>
-      <c r="I66" s="28"/>
-      <c r="J66" s="28"/>
-      <c r="K66" s="28"/>
-      <c r="L66" s="28"/>
+      <c r="B66" s="29"/>
+      <c r="C66" s="29"/>
+      <c r="D66" s="29"/>
+      <c r="E66" s="29"/>
+      <c r="F66" s="29"/>
+      <c r="G66" s="29"/>
+      <c r="H66" s="29"/>
+      <c r="I66" s="29"/>
+      <c r="J66" s="29"/>
+      <c r="K66" s="29"/>
+      <c r="L66" s="29"/>
     </row>
     <row r="67" spans="1:12">
       <c r="A67" s="8">
@@ -5120,36 +5114,36 @@
       </c>
     </row>
     <row r="76" spans="1:12" ht="30" customHeight="1">
-      <c r="A76" s="47" t="s">
+      <c r="A76" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="B76" s="47"/>
-      <c r="C76" s="47"/>
-      <c r="D76" s="47"/>
-      <c r="E76" s="47"/>
-      <c r="F76" s="47"/>
-      <c r="G76" s="47"/>
-      <c r="H76" s="47"/>
-      <c r="I76" s="47"/>
-      <c r="J76" s="47"/>
-      <c r="K76" s="47"/>
-      <c r="L76" s="47"/>
+      <c r="B76" s="30"/>
+      <c r="C76" s="30"/>
+      <c r="D76" s="30"/>
+      <c r="E76" s="30"/>
+      <c r="F76" s="30"/>
+      <c r="G76" s="30"/>
+      <c r="H76" s="30"/>
+      <c r="I76" s="30"/>
+      <c r="J76" s="30"/>
+      <c r="K76" s="30"/>
+      <c r="L76" s="30"/>
     </row>
     <row r="77" spans="1:12">
-      <c r="A77" s="28" t="s">
+      <c r="A77" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="B77" s="28"/>
-      <c r="C77" s="28"/>
-      <c r="D77" s="28"/>
-      <c r="E77" s="28"/>
-      <c r="F77" s="28"/>
-      <c r="G77" s="28"/>
-      <c r="H77" s="28"/>
-      <c r="I77" s="28"/>
-      <c r="J77" s="28"/>
-      <c r="K77" s="28"/>
-      <c r="L77" s="28"/>
+      <c r="B77" s="29"/>
+      <c r="C77" s="29"/>
+      <c r="D77" s="29"/>
+      <c r="E77" s="29"/>
+      <c r="F77" s="29"/>
+      <c r="G77" s="29"/>
+      <c r="H77" s="29"/>
+      <c r="I77" s="29"/>
+      <c r="J77" s="29"/>
+      <c r="K77" s="29"/>
+      <c r="L77" s="29"/>
     </row>
     <row r="78" spans="1:12">
       <c r="A78" s="8">
@@ -5369,7 +5363,7 @@
       <c r="I83" s="8">
         <v>135.79</v>
       </c>
-      <c r="J83" s="46">
+      <c r="J83" s="28">
         <v>1325.58</v>
       </c>
       <c r="K83" s="8">
@@ -5470,20 +5464,20 @@
       <c r="L86" s="8"/>
     </row>
     <row r="87" spans="1:12">
-      <c r="A87" s="28" t="s">
+      <c r="A87" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="B87" s="28"/>
-      <c r="C87" s="28"/>
-      <c r="D87" s="28"/>
-      <c r="E87" s="28"/>
-      <c r="F87" s="28"/>
-      <c r="G87" s="28"/>
-      <c r="H87" s="28"/>
-      <c r="I87" s="28"/>
-      <c r="J87" s="28"/>
-      <c r="K87" s="28"/>
-      <c r="L87" s="28"/>
+      <c r="B87" s="29"/>
+      <c r="C87" s="29"/>
+      <c r="D87" s="29"/>
+      <c r="E87" s="29"/>
+      <c r="F87" s="29"/>
+      <c r="G87" s="29"/>
+      <c r="H87" s="29"/>
+      <c r="I87" s="29"/>
+      <c r="J87" s="29"/>
+      <c r="K87" s="29"/>
+      <c r="L87" s="29"/>
     </row>
     <row r="88" spans="1:12">
       <c r="A88" s="8">
@@ -5697,7 +5691,7 @@
       <c r="G93" s="8"/>
       <c r="H93" s="8"/>
       <c r="I93" s="8"/>
-      <c r="J93" s="46"/>
+      <c r="J93" s="28"/>
       <c r="K93" s="8"/>
       <c r="L93" s="8"/>
     </row>
@@ -5780,20 +5774,20 @@
       <c r="L96" s="8"/>
     </row>
     <row r="97" spans="1:12">
-      <c r="A97" s="28" t="s">
+      <c r="A97" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="B97" s="28"/>
-      <c r="C97" s="28"/>
-      <c r="D97" s="28"/>
-      <c r="E97" s="28"/>
-      <c r="F97" s="28"/>
-      <c r="G97" s="28"/>
-      <c r="H97" s="28"/>
-      <c r="I97" s="28"/>
-      <c r="J97" s="28"/>
-      <c r="K97" s="28"/>
-      <c r="L97" s="28"/>
+      <c r="B97" s="29"/>
+      <c r="C97" s="29"/>
+      <c r="D97" s="29"/>
+      <c r="E97" s="29"/>
+      <c r="F97" s="29"/>
+      <c r="G97" s="29"/>
+      <c r="H97" s="29"/>
+      <c r="I97" s="29"/>
+      <c r="J97" s="29"/>
+      <c r="K97" s="29"/>
+      <c r="L97" s="29"/>
     </row>
     <row r="98" spans="1:12">
       <c r="A98" s="8">
@@ -6051,7 +6045,7 @@
       <c r="I104" s="8">
         <v>310.16199999999998</v>
       </c>
-      <c r="J104" s="46">
+      <c r="J104" s="28">
         <v>580.34</v>
       </c>
       <c r="K104" s="8">
@@ -6114,20 +6108,20 @@
       <c r="L106" s="8"/>
     </row>
     <row r="107" spans="1:12">
-      <c r="A107" s="28" t="s">
+      <c r="A107" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="B107" s="28"/>
-      <c r="C107" s="28"/>
-      <c r="D107" s="28"/>
-      <c r="E107" s="28"/>
-      <c r="F107" s="28"/>
-      <c r="G107" s="28"/>
-      <c r="H107" s="28"/>
-      <c r="I107" s="28"/>
-      <c r="J107" s="28"/>
-      <c r="K107" s="28"/>
-      <c r="L107" s="28"/>
+      <c r="B107" s="29"/>
+      <c r="C107" s="29"/>
+      <c r="D107" s="29"/>
+      <c r="E107" s="29"/>
+      <c r="F107" s="29"/>
+      <c r="G107" s="29"/>
+      <c r="H107" s="29"/>
+      <c r="I107" s="29"/>
+      <c r="J107" s="29"/>
+      <c r="K107" s="29"/>
+      <c r="L107" s="29"/>
     </row>
     <row r="108" spans="1:12">
       <c r="A108" s="8">
@@ -6341,7 +6335,7 @@
       <c r="G113" s="8"/>
       <c r="H113" s="8"/>
       <c r="I113" s="8"/>
-      <c r="J113" s="46"/>
+      <c r="J113" s="28"/>
       <c r="K113" s="8"/>
       <c r="L113" s="8"/>
     </row>
@@ -6423,13 +6417,295 @@
       <c r="K116" s="8"/>
       <c r="L116" s="8"/>
     </row>
+    <row r="117" spans="1:12">
+      <c r="A117" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="B117" s="29"/>
+      <c r="C117" s="29"/>
+      <c r="D117" s="29"/>
+      <c r="E117" s="29"/>
+      <c r="F117" s="29"/>
+      <c r="G117" s="29"/>
+      <c r="H117" s="29"/>
+      <c r="I117" s="29"/>
+      <c r="J117" s="29"/>
+      <c r="K117" s="29"/>
+      <c r="L117" s="29"/>
+    </row>
+    <row r="118" spans="1:12">
+      <c r="A118" s="8">
+        <v>10</v>
+      </c>
+      <c r="B118" s="9">
+        <v>4991</v>
+      </c>
+      <c r="C118" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D118" s="8">
+        <v>2500</v>
+      </c>
+      <c r="E118" s="8">
+        <v>10</v>
+      </c>
+      <c r="F118" s="8">
+        <v>50</v>
+      </c>
+      <c r="G118" s="3">
+        <v>5.0700000000000002E-2</v>
+      </c>
+      <c r="H118" s="3">
+        <v>0.1075</v>
+      </c>
+      <c r="I118" s="3">
+        <v>3.0659999999999998</v>
+      </c>
+      <c r="J118" s="3">
+        <v>58715.29</v>
+      </c>
+      <c r="K118" s="3">
+        <v>6.1310000000000003E-2</v>
+      </c>
+      <c r="L118" s="3">
+        <v>6.0639999999999999E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12">
+      <c r="A119" s="8">
+        <v>50</v>
+      </c>
+      <c r="B119" s="9">
+        <v>22716</v>
+      </c>
+      <c r="C119" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D119" s="8">
+        <v>2500</v>
+      </c>
+      <c r="E119" s="8">
+        <v>10</v>
+      </c>
+      <c r="F119" s="8">
+        <v>50</v>
+      </c>
+      <c r="G119" s="3">
+        <v>5.5199999999999999E-2</v>
+      </c>
+      <c r="H119" s="3">
+        <v>0.11990000000000001</v>
+      </c>
+      <c r="I119" s="3">
+        <v>3.2570000000000001</v>
+      </c>
+      <c r="J119" s="3">
+        <v>55258.59</v>
+      </c>
+      <c r="K119" s="3">
+        <v>6.515E-2</v>
+      </c>
+      <c r="L119" s="3">
+        <v>6.4519999999999994E-2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12">
+      <c r="A120" s="8">
+        <v>100</v>
+      </c>
+      <c r="B120" s="9">
+        <v>40333</v>
+      </c>
+      <c r="C120" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D120" s="8">
+        <v>2500</v>
+      </c>
+      <c r="E120" s="8">
+        <v>10</v>
+      </c>
+      <c r="F120" s="8">
+        <v>50</v>
+      </c>
+      <c r="G120" s="3">
+        <v>7.0099999999999996E-2</v>
+      </c>
+      <c r="H120" s="3">
+        <v>0.41610000000000003</v>
+      </c>
+      <c r="I120" s="3">
+        <v>4.3819999999999997</v>
+      </c>
+      <c r="J120" s="3">
+        <v>41075.83</v>
+      </c>
+      <c r="K120" s="3">
+        <v>8.7639999999999996E-2</v>
+      </c>
+      <c r="L120" s="3">
+        <v>8.2610000000000003E-2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12">
+      <c r="A121" s="8">
+        <v>250</v>
+      </c>
+      <c r="B121" s="9">
+        <v>98113</v>
+      </c>
+      <c r="C121" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D121" s="8">
+        <v>2500</v>
+      </c>
+      <c r="E121" s="8">
+        <v>10</v>
+      </c>
+      <c r="F121" s="8">
+        <v>50</v>
+      </c>
+      <c r="G121" s="3"/>
+      <c r="H121" s="3"/>
+      <c r="I121" s="3"/>
+      <c r="J121" s="3"/>
+      <c r="K121" s="3"/>
+      <c r="L121" s="3"/>
+    </row>
+    <row r="122" spans="1:12">
+      <c r="A122" s="8">
+        <v>500</v>
+      </c>
+      <c r="B122" s="9">
+        <v>191502</v>
+      </c>
+      <c r="C122" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D122" s="8">
+        <v>2500</v>
+      </c>
+      <c r="E122" s="8">
+        <v>10</v>
+      </c>
+      <c r="F122" s="8">
+        <v>50</v>
+      </c>
+      <c r="G122" s="3"/>
+      <c r="H122" s="3"/>
+      <c r="I122" s="3"/>
+      <c r="J122" s="3"/>
+      <c r="K122" s="3"/>
+      <c r="L122" s="3"/>
+    </row>
+    <row r="123" spans="1:12">
+      <c r="A123" s="8">
+        <v>1000</v>
+      </c>
+      <c r="B123" s="9">
+        <v>375114</v>
+      </c>
+      <c r="C123" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D123" s="8">
+        <v>2500</v>
+      </c>
+      <c r="E123" s="8">
+        <v>10</v>
+      </c>
+      <c r="F123" s="8">
+        <v>50</v>
+      </c>
+      <c r="G123" s="3"/>
+      <c r="H123" s="3"/>
+      <c r="I123" s="3"/>
+      <c r="J123" s="3"/>
+      <c r="K123" s="3"/>
+      <c r="L123" s="3"/>
+    </row>
+    <row r="124" spans="1:12">
+      <c r="A124" s="5">
+        <v>1500</v>
+      </c>
+      <c r="B124" s="7">
+        <v>550078</v>
+      </c>
+      <c r="C124" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D124" s="5">
+        <v>2500</v>
+      </c>
+      <c r="E124" s="8">
+        <v>10</v>
+      </c>
+      <c r="F124" s="8">
+        <v>50</v>
+      </c>
+      <c r="G124" s="3"/>
+      <c r="H124" s="3"/>
+      <c r="I124" s="3"/>
+      <c r="J124" s="3"/>
+      <c r="K124" s="3"/>
+      <c r="L124" s="3"/>
+    </row>
+    <row r="125" spans="1:12">
+      <c r="A125" s="5">
+        <v>2000</v>
+      </c>
+      <c r="B125" s="7">
+        <v>725515</v>
+      </c>
+      <c r="C125" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D125" s="5">
+        <v>2500</v>
+      </c>
+      <c r="E125" s="8">
+        <v>10</v>
+      </c>
+      <c r="F125" s="8">
+        <v>50</v>
+      </c>
+      <c r="G125" s="3"/>
+      <c r="H125" s="3"/>
+      <c r="I125" s="3"/>
+      <c r="J125" s="3"/>
+      <c r="K125" s="3"/>
+      <c r="L125" s="3"/>
+    </row>
+    <row r="126" spans="1:12">
+      <c r="A126" s="5">
+        <v>2500</v>
+      </c>
+      <c r="B126" s="7">
+        <v>900517</v>
+      </c>
+      <c r="C126" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D126" s="5">
+        <v>2500</v>
+      </c>
+      <c r="E126" s="8">
+        <v>10</v>
+      </c>
+      <c r="F126" s="8">
+        <v>50</v>
+      </c>
+      <c r="G126" s="3"/>
+      <c r="H126" s="3"/>
+      <c r="I126" s="3"/>
+      <c r="J126" s="3"/>
+      <c r="K126" s="3"/>
+      <c r="L126" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="A77:L77"/>
-    <mergeCell ref="A97:L97"/>
-    <mergeCell ref="A76:L76"/>
-    <mergeCell ref="A87:L87"/>
-    <mergeCell ref="A107:L107"/>
+  <mergeCells count="21">
+    <mergeCell ref="A117:L117"/>
     <mergeCell ref="A66:L66"/>
     <mergeCell ref="G57:L64"/>
     <mergeCell ref="A1:C1"/>
@@ -6445,6 +6721,11 @@
     <mergeCell ref="A36:L36"/>
     <mergeCell ref="A31:L31"/>
     <mergeCell ref="A24:L24"/>
+    <mergeCell ref="A77:L77"/>
+    <mergeCell ref="A97:L97"/>
+    <mergeCell ref="A76:L76"/>
+    <mergeCell ref="A87:L87"/>
+    <mergeCell ref="A107:L107"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6475,11 +6756,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
       <c r="D1" s="24"/>
       <c r="E1" s="24"/>
     </row>
@@ -6490,28 +6771,28 @@
       <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:14" ht="15.75">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="44" t="s">
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="45"/>
-      <c r="F3" s="42" t="s">
+      <c r="E3" s="47"/>
+      <c r="F3" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42" t="s">
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="6" t="s">
@@ -6558,22 +6839,22 @@
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="8">
@@ -6961,11 +7242,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
       <c r="D1" s="26"/>
       <c r="E1" s="26"/>
     </row>
@@ -6976,28 +7257,28 @@
       <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:14" ht="15.75">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="44" t="s">
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="45"/>
-      <c r="F3" s="42" t="s">
+      <c r="E3" s="47"/>
+      <c r="F3" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42" t="s">
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="6" t="s">
@@ -7044,22 +7325,22 @@
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
+      <c r="A5" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="8">
@@ -7366,11 +7647,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
       <c r="D1" s="25"/>
       <c r="E1" s="25"/>
     </row>
@@ -7381,28 +7662,28 @@
       <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:14" ht="15.75">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="44" t="s">
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="45"/>
-      <c r="F3" s="42" t="s">
+      <c r="E3" s="47"/>
+      <c r="F3" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42" t="s">
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="6" t="s">
@@ -7449,22 +7730,22 @@
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="8">

</xml_diff>

<commit_message>
Added initial BSBM results from early 0.4.2 builds of dotNetRDF, already showing promising improvements re: scalability
</commit_message>
<xml_diff>
--- a/Benchmarks/dotNetRDF BSBM Benchmark.xlsx
+++ b/Benchmarks/dotNetRDF BSBM Benchmark.xlsx
@@ -2654,8 +2654,8 @@
   <dimension ref="A1:L126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G121" sqref="G121"/>
+      <pane ySplit="4" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G125" sqref="G125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6566,12 +6566,24 @@
       <c r="F121" s="8">
         <v>50</v>
       </c>
-      <c r="G121" s="3"/>
-      <c r="H121" s="3"/>
-      <c r="I121" s="3"/>
-      <c r="J121" s="3"/>
-      <c r="K121" s="3"/>
-      <c r="L121" s="3"/>
+      <c r="G121" s="3">
+        <v>0.1643</v>
+      </c>
+      <c r="H121" s="3">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="I121" s="3">
+        <v>9.3620000000000001</v>
+      </c>
+      <c r="J121" s="3">
+        <v>19225.830000000002</v>
+      </c>
+      <c r="K121" s="3">
+        <v>0.18725</v>
+      </c>
+      <c r="L121" s="3">
+        <v>0.18583</v>
+      </c>
     </row>
     <row r="122" spans="1:12">
       <c r="A122" s="8">
@@ -6592,12 +6604,24 @@
       <c r="F122" s="8">
         <v>50</v>
       </c>
-      <c r="G122" s="3"/>
-      <c r="H122" s="3"/>
-      <c r="I122" s="3"/>
-      <c r="J122" s="3"/>
-      <c r="K122" s="3"/>
-      <c r="L122" s="3"/>
+      <c r="G122" s="3">
+        <v>0.51680000000000004</v>
+      </c>
+      <c r="H122" s="3">
+        <v>0.8448</v>
+      </c>
+      <c r="I122" s="3">
+        <v>28.271999999999998</v>
+      </c>
+      <c r="J122" s="3">
+        <v>6366.7</v>
+      </c>
+      <c r="K122" s="3">
+        <v>0.56544000000000005</v>
+      </c>
+      <c r="L122" s="3">
+        <v>0.56186999999999998</v>
+      </c>
     </row>
     <row r="123" spans="1:12">
       <c r="A123" s="8">
@@ -6618,12 +6642,24 @@
       <c r="F123" s="8">
         <v>50</v>
       </c>
-      <c r="G123" s="3"/>
-      <c r="H123" s="3"/>
-      <c r="I123" s="3"/>
-      <c r="J123" s="3"/>
-      <c r="K123" s="3"/>
-      <c r="L123" s="3"/>
+      <c r="G123" s="3">
+        <v>1.8153999999999999</v>
+      </c>
+      <c r="H123" s="3">
+        <v>3.1198999999999999</v>
+      </c>
+      <c r="I123" s="3">
+        <v>97.835999999999999</v>
+      </c>
+      <c r="J123" s="3">
+        <v>1839.81</v>
+      </c>
+      <c r="K123" s="3">
+        <v>1.95672</v>
+      </c>
+      <c r="L123" s="3">
+        <v>1.9471499999999999</v>
+      </c>
     </row>
     <row r="124" spans="1:12">
       <c r="A124" s="5">
@@ -6644,12 +6680,24 @@
       <c r="F124" s="8">
         <v>50</v>
       </c>
-      <c r="G124" s="3"/>
-      <c r="H124" s="3"/>
-      <c r="I124" s="3"/>
-      <c r="J124" s="3"/>
-      <c r="K124" s="3"/>
-      <c r="L124" s="3"/>
+      <c r="G124" s="3">
+        <v>4.2595999999999998</v>
+      </c>
+      <c r="H124" s="3">
+        <v>5.6853999999999996</v>
+      </c>
+      <c r="I124" s="3">
+        <v>232.38200000000001</v>
+      </c>
+      <c r="J124" s="3">
+        <v>774.59</v>
+      </c>
+      <c r="K124" s="3">
+        <v>4.64764</v>
+      </c>
+      <c r="L124" s="3">
+        <v>4.6351300000000002</v>
+      </c>
     </row>
     <row r="125" spans="1:12">
       <c r="A125" s="5">

</xml_diff>

<commit_message>
Tried a new SPARQL optimisation but found it didn't work as well as expected and may actually cause dud results so disabled again
</commit_message>
<xml_diff>
--- a/Benchmarks/dotNetRDF BSBM Benchmark.xlsx
+++ b/Benchmarks/dotNetRDF BSBM Benchmark.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="59">
   <si>
     <t>BSBM Benchmarks</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>Leviathan Engine - Version 0.4.2 using Default Optimiser</t>
+  </si>
+  <si>
+    <t>Leviathan Engine - Version 0.4.2 (Non-rigorous optimisation) using Default Optimiser</t>
   </si>
 </sst>
 </file>
@@ -486,9 +489,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -533,6 +533,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1130,11 +1133,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="56537472"/>
-        <c:axId val="56539008"/>
+        <c:axId val="77733248"/>
+        <c:axId val="77743232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="56537472"/>
+        <c:axId val="77733248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1142,14 +1145,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56539008"/>
+        <c:crossAx val="77743232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="56539008"/>
+        <c:axId val="77743232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1175,7 +1178,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56537472"/>
+        <c:crossAx val="77733248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1187,7 +1190,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1525,11 +1528,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="56871168"/>
-        <c:axId val="56881152"/>
+        <c:axId val="77923840"/>
+        <c:axId val="77925376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="56871168"/>
+        <c:axId val="77923840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1537,14 +1540,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56881152"/>
+        <c:crossAx val="77925376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="56881152"/>
+        <c:axId val="77925376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1570,7 +1573,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56871168"/>
+        <c:crossAx val="77923840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1582,7 +1585,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1788,25 +1791,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="57168640"/>
-        <c:axId val="57170176"/>
+        <c:axId val="77971456"/>
+        <c:axId val="77972992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="57168640"/>
+        <c:axId val="77971456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57170176"/>
+        <c:crossAx val="77972992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57170176"/>
+        <c:axId val="77972992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1831,7 +1834,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57168640"/>
+        <c:crossAx val="77971456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1843,7 +1846,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2175,25 +2178,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="62686336"/>
-        <c:axId val="62687872"/>
+        <c:axId val="78127488"/>
+        <c:axId val="78129024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="62686336"/>
+        <c:axId val="78127488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62687872"/>
+        <c:crossAx val="78129024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62687872"/>
+        <c:axId val="78129024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2218,7 +2221,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62686336"/>
+        <c:crossAx val="78127488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2230,7 +2233,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2651,18 +2654,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L126"/>
+  <dimension ref="A1:L136"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G125" sqref="G125"/>
+      <pane ySplit="4" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M130" sqref="M130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" customWidth="1"/>
@@ -2674,34 +2677,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1">
       <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="15.75">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44" t="s">
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44" t="s">
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="6" t="s">
@@ -2742,20 +2745,20 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="43"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="42"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="5">
@@ -2834,20 +2837,20 @@
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="43"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="42"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="8">
@@ -3002,20 +3005,20 @@
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="42"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="42"/>
-      <c r="K13" s="42"/>
-      <c r="L13" s="43"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="42"/>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="5">
@@ -3246,20 +3249,20 @@
       </c>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="42"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="42"/>
-      <c r="L20" s="43"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="41"/>
+      <c r="L20" s="42"/>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="8">
@@ -3376,20 +3379,20 @@
       </c>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="42"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
-      <c r="K24" s="42"/>
-      <c r="L24" s="43"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="41"/>
+      <c r="J24" s="41"/>
+      <c r="K24" s="41"/>
+      <c r="L24" s="42"/>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="8">
@@ -3620,20 +3623,20 @@
       </c>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="41" t="s">
+      <c r="A31" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="42"/>
-      <c r="C31" s="42"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="42"/>
-      <c r="J31" s="42"/>
-      <c r="K31" s="42"/>
-      <c r="L31" s="43"/>
+      <c r="B31" s="41"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="41"/>
+      <c r="J31" s="41"/>
+      <c r="K31" s="41"/>
+      <c r="L31" s="42"/>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="8">
@@ -3788,20 +3791,20 @@
       </c>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="41" t="s">
+      <c r="A36" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="42"/>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="42"/>
-      <c r="G36" s="42"/>
-      <c r="H36" s="42"/>
-      <c r="I36" s="42"/>
-      <c r="J36" s="42"/>
-      <c r="K36" s="42"/>
-      <c r="L36" s="43"/>
+      <c r="B36" s="41"/>
+      <c r="C36" s="41"/>
+      <c r="D36" s="41"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
+      <c r="G36" s="41"/>
+      <c r="H36" s="41"/>
+      <c r="I36" s="41"/>
+      <c r="J36" s="41"/>
+      <c r="K36" s="41"/>
+      <c r="L36" s="42"/>
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="8">
@@ -4492,20 +4495,20 @@
       <c r="L55" s="8"/>
     </row>
     <row r="56" spans="1:12">
-      <c r="A56" s="45" t="s">
+      <c r="A56" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="B56" s="45"/>
-      <c r="C56" s="45"/>
-      <c r="D56" s="45"/>
-      <c r="E56" s="45"/>
-      <c r="F56" s="45"/>
-      <c r="G56" s="45"/>
-      <c r="H56" s="45"/>
-      <c r="I56" s="45"/>
-      <c r="J56" s="45"/>
-      <c r="K56" s="45"/>
-      <c r="L56" s="45"/>
+      <c r="B56" s="44"/>
+      <c r="C56" s="44"/>
+      <c r="D56" s="44"/>
+      <c r="E56" s="44"/>
+      <c r="F56" s="44"/>
+      <c r="G56" s="44"/>
+      <c r="H56" s="44"/>
+      <c r="I56" s="44"/>
+      <c r="J56" s="44"/>
+      <c r="K56" s="44"/>
+      <c r="L56" s="44"/>
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="19">
@@ -4526,14 +4529,14 @@
       <c r="F57" s="19">
         <v>50</v>
       </c>
-      <c r="G57" s="31" t="s">
+      <c r="G57" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="H57" s="32"/>
-      <c r="I57" s="32"/>
-      <c r="J57" s="32"/>
-      <c r="K57" s="32"/>
-      <c r="L57" s="33"/>
+      <c r="H57" s="31"/>
+      <c r="I57" s="31"/>
+      <c r="J57" s="31"/>
+      <c r="K57" s="31"/>
+      <c r="L57" s="32"/>
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="19">
@@ -4554,12 +4557,12 @@
       <c r="F58" s="19">
         <v>50</v>
       </c>
-      <c r="G58" s="34"/>
-      <c r="H58" s="35"/>
-      <c r="I58" s="35"/>
-      <c r="J58" s="35"/>
-      <c r="K58" s="35"/>
-      <c r="L58" s="36"/>
+      <c r="G58" s="33"/>
+      <c r="H58" s="34"/>
+      <c r="I58" s="34"/>
+      <c r="J58" s="34"/>
+      <c r="K58" s="34"/>
+      <c r="L58" s="35"/>
     </row>
     <row r="59" spans="1:12">
       <c r="A59" s="19">
@@ -4580,12 +4583,12 @@
       <c r="F59" s="19">
         <v>50</v>
       </c>
-      <c r="G59" s="34"/>
-      <c r="H59" s="35"/>
-      <c r="I59" s="35"/>
-      <c r="J59" s="35"/>
-      <c r="K59" s="35"/>
-      <c r="L59" s="36"/>
+      <c r="G59" s="33"/>
+      <c r="H59" s="34"/>
+      <c r="I59" s="34"/>
+      <c r="J59" s="34"/>
+      <c r="K59" s="34"/>
+      <c r="L59" s="35"/>
     </row>
     <row r="60" spans="1:12">
       <c r="A60" s="19">
@@ -4606,12 +4609,12 @@
       <c r="F60" s="19">
         <v>50</v>
       </c>
-      <c r="G60" s="34"/>
-      <c r="H60" s="35"/>
-      <c r="I60" s="35"/>
-      <c r="J60" s="35"/>
-      <c r="K60" s="35"/>
-      <c r="L60" s="36"/>
+      <c r="G60" s="33"/>
+      <c r="H60" s="34"/>
+      <c r="I60" s="34"/>
+      <c r="J60" s="34"/>
+      <c r="K60" s="34"/>
+      <c r="L60" s="35"/>
     </row>
     <row r="61" spans="1:12">
       <c r="A61" s="19">
@@ -4632,12 +4635,12 @@
       <c r="F61" s="19">
         <v>50</v>
       </c>
-      <c r="G61" s="34"/>
-      <c r="H61" s="35"/>
-      <c r="I61" s="35"/>
-      <c r="J61" s="35"/>
-      <c r="K61" s="35"/>
-      <c r="L61" s="36"/>
+      <c r="G61" s="33"/>
+      <c r="H61" s="34"/>
+      <c r="I61" s="34"/>
+      <c r="J61" s="34"/>
+      <c r="K61" s="34"/>
+      <c r="L61" s="35"/>
     </row>
     <row r="62" spans="1:12">
       <c r="A62" s="19">
@@ -4658,12 +4661,12 @@
       <c r="F62" s="19">
         <v>50</v>
       </c>
-      <c r="G62" s="34"/>
-      <c r="H62" s="35"/>
-      <c r="I62" s="35"/>
-      <c r="J62" s="35"/>
-      <c r="K62" s="35"/>
-      <c r="L62" s="36"/>
+      <c r="G62" s="33"/>
+      <c r="H62" s="34"/>
+      <c r="I62" s="34"/>
+      <c r="J62" s="34"/>
+      <c r="K62" s="34"/>
+      <c r="L62" s="35"/>
     </row>
     <row r="63" spans="1:12">
       <c r="A63" s="22">
@@ -4684,12 +4687,12 @@
       <c r="F63" s="19">
         <v>50</v>
       </c>
-      <c r="G63" s="34"/>
-      <c r="H63" s="35"/>
-      <c r="I63" s="35"/>
-      <c r="J63" s="35"/>
-      <c r="K63" s="35"/>
-      <c r="L63" s="36"/>
+      <c r="G63" s="33"/>
+      <c r="H63" s="34"/>
+      <c r="I63" s="34"/>
+      <c r="J63" s="34"/>
+      <c r="K63" s="34"/>
+      <c r="L63" s="35"/>
     </row>
     <row r="64" spans="1:12">
       <c r="A64" s="22">
@@ -4710,12 +4713,12 @@
       <c r="F64" s="19">
         <v>50</v>
       </c>
-      <c r="G64" s="37"/>
-      <c r="H64" s="38"/>
-      <c r="I64" s="38"/>
-      <c r="J64" s="38"/>
-      <c r="K64" s="38"/>
-      <c r="L64" s="39"/>
+      <c r="G64" s="36"/>
+      <c r="H64" s="37"/>
+      <c r="I64" s="37"/>
+      <c r="J64" s="37"/>
+      <c r="K64" s="37"/>
+      <c r="L64" s="38"/>
     </row>
     <row r="65" spans="1:12">
       <c r="A65" s="22">
@@ -5114,20 +5117,20 @@
       </c>
     </row>
     <row r="76" spans="1:12" ht="30" customHeight="1">
-      <c r="A76" s="30" t="s">
+      <c r="A76" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="B76" s="30"/>
-      <c r="C76" s="30"/>
-      <c r="D76" s="30"/>
-      <c r="E76" s="30"/>
-      <c r="F76" s="30"/>
-      <c r="G76" s="30"/>
-      <c r="H76" s="30"/>
-      <c r="I76" s="30"/>
-      <c r="J76" s="30"/>
-      <c r="K76" s="30"/>
-      <c r="L76" s="30"/>
+      <c r="B76" s="45"/>
+      <c r="C76" s="45"/>
+      <c r="D76" s="45"/>
+      <c r="E76" s="45"/>
+      <c r="F76" s="45"/>
+      <c r="G76" s="45"/>
+      <c r="H76" s="45"/>
+      <c r="I76" s="45"/>
+      <c r="J76" s="45"/>
+      <c r="K76" s="45"/>
+      <c r="L76" s="45"/>
     </row>
     <row r="77" spans="1:12">
       <c r="A77" s="29" t="s">
@@ -6751,8 +6754,336 @@
       <c r="K126" s="3"/>
       <c r="L126" s="3"/>
     </row>
+    <row r="127" spans="1:12">
+      <c r="A127" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B127" s="29"/>
+      <c r="C127" s="29"/>
+      <c r="D127" s="29"/>
+      <c r="E127" s="29"/>
+      <c r="F127" s="29"/>
+      <c r="G127" s="29"/>
+      <c r="H127" s="29"/>
+      <c r="I127" s="29"/>
+      <c r="J127" s="29"/>
+      <c r="K127" s="29"/>
+      <c r="L127" s="29"/>
+    </row>
+    <row r="128" spans="1:12">
+      <c r="A128" s="8">
+        <v>10</v>
+      </c>
+      <c r="B128" s="9">
+        <v>4991</v>
+      </c>
+      <c r="C128" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D128" s="8">
+        <v>2500</v>
+      </c>
+      <c r="E128" s="8">
+        <v>10</v>
+      </c>
+      <c r="F128" s="8">
+        <v>50</v>
+      </c>
+      <c r="G128" s="3">
+        <v>4.6100000000000002E-2</v>
+      </c>
+      <c r="H128" s="3">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="I128" s="3">
+        <v>2.8639999999999999</v>
+      </c>
+      <c r="J128" s="3">
+        <v>62856.24</v>
+      </c>
+      <c r="K128" s="3">
+        <v>5.7270000000000001E-2</v>
+      </c>
+      <c r="L128" s="3">
+        <v>5.6890000000000003E-2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12">
+      <c r="A129" s="8">
+        <v>50</v>
+      </c>
+      <c r="B129" s="9">
+        <v>22716</v>
+      </c>
+      <c r="C129" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D129" s="8">
+        <v>2500</v>
+      </c>
+      <c r="E129" s="8">
+        <v>10</v>
+      </c>
+      <c r="F129" s="8">
+        <v>50</v>
+      </c>
+      <c r="G129" s="3">
+        <v>5.2200000000000003E-2</v>
+      </c>
+      <c r="H129" s="3">
+        <v>7.6899999999999996E-2</v>
+      </c>
+      <c r="I129" s="3">
+        <v>3.1030000000000002</v>
+      </c>
+      <c r="J129" s="3">
+        <v>58004.74</v>
+      </c>
+      <c r="K129" s="3">
+        <v>6.2059999999999997E-2</v>
+      </c>
+      <c r="L129" s="3">
+        <v>6.1809999999999997E-2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12">
+      <c r="A130" s="8">
+        <v>100</v>
+      </c>
+      <c r="B130" s="9">
+        <v>40333</v>
+      </c>
+      <c r="C130" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D130" s="8">
+        <v>2500</v>
+      </c>
+      <c r="E130" s="8">
+        <v>10</v>
+      </c>
+      <c r="F130" s="8">
+        <v>50</v>
+      </c>
+      <c r="G130" s="3">
+        <v>6.5799999999999997E-2</v>
+      </c>
+      <c r="H130" s="3">
+        <v>0.11020000000000001</v>
+      </c>
+      <c r="I130" s="3">
+        <v>3.8450000000000002</v>
+      </c>
+      <c r="J130" s="3">
+        <v>46809.59</v>
+      </c>
+      <c r="K130" s="3">
+        <v>7.6910000000000006E-2</v>
+      </c>
+      <c r="L130" s="3">
+        <v>7.6490000000000002E-2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12">
+      <c r="A131" s="8">
+        <v>250</v>
+      </c>
+      <c r="B131" s="9">
+        <v>98113</v>
+      </c>
+      <c r="C131" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D131" s="8">
+        <v>2500</v>
+      </c>
+      <c r="E131" s="8">
+        <v>10</v>
+      </c>
+      <c r="F131" s="8">
+        <v>50</v>
+      </c>
+      <c r="G131" s="3">
+        <v>0.16</v>
+      </c>
+      <c r="H131" s="3">
+        <v>0.56169999999999998</v>
+      </c>
+      <c r="I131" s="3">
+        <v>9.4169999999999998</v>
+      </c>
+      <c r="J131" s="3">
+        <v>19115.05</v>
+      </c>
+      <c r="K131" s="3">
+        <v>0.18833</v>
+      </c>
+      <c r="L131" s="3">
+        <v>0.18359</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12">
+      <c r="A132" s="8">
+        <v>500</v>
+      </c>
+      <c r="B132" s="9">
+        <v>191502</v>
+      </c>
+      <c r="C132" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D132" s="8">
+        <v>2500</v>
+      </c>
+      <c r="E132" s="8">
+        <v>10</v>
+      </c>
+      <c r="F132" s="8">
+        <v>50</v>
+      </c>
+      <c r="G132" s="3">
+        <v>0.48730000000000001</v>
+      </c>
+      <c r="H132" s="3">
+        <v>1.4349000000000001</v>
+      </c>
+      <c r="I132" s="3">
+        <v>28.01</v>
+      </c>
+      <c r="J132" s="3">
+        <v>6426.31</v>
+      </c>
+      <c r="K132" s="3">
+        <v>0.56020000000000003</v>
+      </c>
+      <c r="L132" s="3">
+        <v>0.54986000000000002</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12">
+      <c r="A133" s="8">
+        <v>1000</v>
+      </c>
+      <c r="B133" s="9">
+        <v>375114</v>
+      </c>
+      <c r="C133" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D133" s="8">
+        <v>2500</v>
+      </c>
+      <c r="E133" s="8">
+        <v>10</v>
+      </c>
+      <c r="F133" s="8">
+        <v>50</v>
+      </c>
+      <c r="G133" s="3">
+        <v>1.8193999999999999</v>
+      </c>
+      <c r="H133" s="3">
+        <v>3.9373999999999998</v>
+      </c>
+      <c r="I133" s="3">
+        <v>106.005</v>
+      </c>
+      <c r="J133" s="3">
+        <v>1698.04</v>
+      </c>
+      <c r="K133" s="3">
+        <v>2.1200899999999998</v>
+      </c>
+      <c r="L133" s="3">
+        <v>2.0813299999999999</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12">
+      <c r="A134" s="5">
+        <v>1500</v>
+      </c>
+      <c r="B134" s="7">
+        <v>550078</v>
+      </c>
+      <c r="C134" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D134" s="5">
+        <v>2500</v>
+      </c>
+      <c r="E134" s="8">
+        <v>10</v>
+      </c>
+      <c r="F134" s="8">
+        <v>50</v>
+      </c>
+      <c r="G134" s="3"/>
+      <c r="H134" s="3"/>
+      <c r="I134" s="3"/>
+      <c r="J134" s="3"/>
+      <c r="K134" s="3"/>
+      <c r="L134" s="3"/>
+    </row>
+    <row r="135" spans="1:12">
+      <c r="A135" s="5">
+        <v>2000</v>
+      </c>
+      <c r="B135" s="7">
+        <v>725515</v>
+      </c>
+      <c r="C135" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D135" s="5">
+        <v>2500</v>
+      </c>
+      <c r="E135" s="8">
+        <v>10</v>
+      </c>
+      <c r="F135" s="8">
+        <v>50</v>
+      </c>
+      <c r="G135" s="3"/>
+      <c r="H135" s="3"/>
+      <c r="I135" s="3"/>
+      <c r="J135" s="3"/>
+      <c r="K135" s="3"/>
+      <c r="L135" s="3"/>
+    </row>
+    <row r="136" spans="1:12">
+      <c r="A136" s="5">
+        <v>2500</v>
+      </c>
+      <c r="B136" s="7">
+        <v>900517</v>
+      </c>
+      <c r="C136" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D136" s="5">
+        <v>2500</v>
+      </c>
+      <c r="E136" s="8">
+        <v>10</v>
+      </c>
+      <c r="F136" s="8">
+        <v>50</v>
+      </c>
+      <c r="G136" s="3"/>
+      <c r="H136" s="3"/>
+      <c r="I136" s="3"/>
+      <c r="J136" s="3"/>
+      <c r="K136" s="3"/>
+      <c r="L136" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="22">
+    <mergeCell ref="A127:L127"/>
+    <mergeCell ref="A77:L77"/>
+    <mergeCell ref="A97:L97"/>
+    <mergeCell ref="A76:L76"/>
+    <mergeCell ref="A87:L87"/>
+    <mergeCell ref="A107:L107"/>
     <mergeCell ref="A117:L117"/>
     <mergeCell ref="A66:L66"/>
     <mergeCell ref="G57:L64"/>
@@ -6769,11 +7100,6 @@
     <mergeCell ref="A36:L36"/>
     <mergeCell ref="A31:L31"/>
     <mergeCell ref="A24:L24"/>
-    <mergeCell ref="A77:L77"/>
-    <mergeCell ref="A97:L97"/>
-    <mergeCell ref="A76:L76"/>
-    <mergeCell ref="A87:L87"/>
-    <mergeCell ref="A107:L107"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6804,11 +7130,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
       <c r="D1" s="24"/>
       <c r="E1" s="24"/>
     </row>
@@ -6819,28 +7145,28 @@
       <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:14" ht="15.75">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
       <c r="D3" s="46" t="s">
         <v>44</v>
       </c>
       <c r="E3" s="47"/>
-      <c r="F3" s="44" t="s">
+      <c r="F3" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44" t="s">
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="6" t="s">
@@ -7290,11 +7616,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
       <c r="D1" s="26"/>
       <c r="E1" s="26"/>
     </row>
@@ -7305,28 +7631,28 @@
       <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:14" ht="15.75">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
       <c r="D3" s="46" t="s">
         <v>44</v>
       </c>
       <c r="E3" s="47"/>
-      <c r="F3" s="44" t="s">
+      <c r="F3" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44" t="s">
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="6" t="s">
@@ -7695,11 +8021,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
       <c r="D1" s="25"/>
       <c r="E1" s="25"/>
     </row>
@@ -7710,28 +8036,28 @@
       <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:14" ht="15.75">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
       <c r="D3" s="46" t="s">
         <v>44</v>
       </c>
       <c r="E3" s="47"/>
-      <c r="F3" s="44" t="s">
+      <c r="F3" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44" t="s">
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="6" t="s">

</xml_diff>

<commit_message>
Added basic parallel query evaluation support
</commit_message>
<xml_diff>
--- a/Benchmarks/dotNetRDF BSBM Benchmark.xlsx
+++ b/Benchmarks/dotNetRDF BSBM Benchmark.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="61">
   <si>
     <t>BSBM Benchmarks</t>
   </si>
@@ -192,10 +192,16 @@
     <t>Leviathan Engine - Version 0.4.1 using Statistics Optimiser with 4 Clients</t>
   </si>
   <si>
-    <t>Leviathan Engine - Version 0.4.2 using Default Optimiser</t>
+    <t>Leviathan Engine - Version 0.4.2 (Non-rigorous evaluation) using Default Optimiser</t>
   </si>
   <si>
-    <t>Leviathan Engine - Version 0.4.2 (Non-rigorous optimisation) using Default Optimiser</t>
+    <t>Results here are considered suspect as analysis suggested they were incorrect.  Non-rigorous evaluation strategy has been removed from the engine</t>
+  </si>
+  <si>
+    <t>Leviathan Engine - Version 0.4.2 (Basic Optimisations) using Default Optimiser</t>
+  </si>
+  <si>
+    <t>Leviathan Engine - Version 0.4.2 (With Identity Filter optimisation enabled) using Default Optimiser</t>
   </si>
 </sst>
 </file>
@@ -412,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -489,6 +495,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -534,14 +543,35 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1133,11 +1163,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="77733248"/>
-        <c:axId val="77743232"/>
+        <c:axId val="93539712"/>
+        <c:axId val="93549696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="77733248"/>
+        <c:axId val="93539712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1145,14 +1175,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77743232"/>
+        <c:crossAx val="93549696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77743232"/>
+        <c:axId val="93549696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1178,7 +1208,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77733248"/>
+        <c:crossAx val="93539712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1190,7 +1220,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1528,11 +1558,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="77923840"/>
-        <c:axId val="77925376"/>
+        <c:axId val="93722112"/>
+        <c:axId val="93723648"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="77923840"/>
+        <c:axId val="93722112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1540,14 +1570,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77925376"/>
+        <c:crossAx val="93723648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77925376"/>
+        <c:axId val="93723648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1573,7 +1603,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77923840"/>
+        <c:crossAx val="93722112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1585,7 +1615,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1791,25 +1821,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="77971456"/>
-        <c:axId val="77972992"/>
+        <c:axId val="93769728"/>
+        <c:axId val="93771264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="77971456"/>
+        <c:axId val="93769728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77972992"/>
+        <c:crossAx val="93771264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77972992"/>
+        <c:axId val="93771264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1834,7 +1864,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77971456"/>
+        <c:crossAx val="93769728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1846,7 +1876,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2178,25 +2208,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="78127488"/>
-        <c:axId val="78129024"/>
+        <c:axId val="97010048"/>
+        <c:axId val="97011584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="78127488"/>
+        <c:axId val="97010048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78129024"/>
+        <c:crossAx val="97011584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78129024"/>
+        <c:axId val="97011584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2221,7 +2251,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78127488"/>
+        <c:crossAx val="97010048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2233,7 +2263,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2654,11 +2684,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L136"/>
+  <dimension ref="A1:L146"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M130" sqref="M130"/>
+      <selection pane="bottomLeft" activeCell="A137" sqref="A137:L137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2677,34 +2707,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1">
       <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="15.75">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43" t="s">
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43" t="s">
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="6" t="s">
@@ -2745,20 +2775,20 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="42"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="43"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="5">
@@ -2837,20 +2867,20 @@
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="42"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="43"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="8">
@@ -3005,20 +3035,20 @@
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="42"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="43"/>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="5">
@@ -3249,20 +3279,20 @@
       </c>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="40" t="s">
+      <c r="A20" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="41"/>
-      <c r="L20" s="42"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="43"/>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="8">
@@ -3379,20 +3409,20 @@
       </c>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="40" t="s">
+      <c r="A24" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="41"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="41"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="41"/>
-      <c r="J24" s="41"/>
-      <c r="K24" s="41"/>
-      <c r="L24" s="42"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="43"/>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="8">
@@ -3623,20 +3653,20 @@
       </c>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="40" t="s">
+      <c r="A31" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="41"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="41"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="41"/>
-      <c r="I31" s="41"/>
-      <c r="J31" s="41"/>
-      <c r="K31" s="41"/>
-      <c r="L31" s="42"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="42"/>
+      <c r="J31" s="42"/>
+      <c r="K31" s="42"/>
+      <c r="L31" s="43"/>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="8">
@@ -3791,20 +3821,20 @@
       </c>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="40" t="s">
+      <c r="A36" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="41"/>
-      <c r="C36" s="41"/>
-      <c r="D36" s="41"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
-      <c r="G36" s="41"/>
-      <c r="H36" s="41"/>
-      <c r="I36" s="41"/>
-      <c r="J36" s="41"/>
-      <c r="K36" s="41"/>
-      <c r="L36" s="42"/>
+      <c r="B36" s="42"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="42"/>
+      <c r="G36" s="42"/>
+      <c r="H36" s="42"/>
+      <c r="I36" s="42"/>
+      <c r="J36" s="42"/>
+      <c r="K36" s="42"/>
+      <c r="L36" s="43"/>
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="8">
@@ -4495,20 +4525,20 @@
       <c r="L55" s="8"/>
     </row>
     <row r="56" spans="1:12">
-      <c r="A56" s="44" t="s">
+      <c r="A56" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="B56" s="44"/>
-      <c r="C56" s="44"/>
-      <c r="D56" s="44"/>
-      <c r="E56" s="44"/>
-      <c r="F56" s="44"/>
-      <c r="G56" s="44"/>
-      <c r="H56" s="44"/>
-      <c r="I56" s="44"/>
-      <c r="J56" s="44"/>
-      <c r="K56" s="44"/>
-      <c r="L56" s="44"/>
+      <c r="B56" s="45"/>
+      <c r="C56" s="45"/>
+      <c r="D56" s="45"/>
+      <c r="E56" s="45"/>
+      <c r="F56" s="45"/>
+      <c r="G56" s="45"/>
+      <c r="H56" s="45"/>
+      <c r="I56" s="45"/>
+      <c r="J56" s="45"/>
+      <c r="K56" s="45"/>
+      <c r="L56" s="45"/>
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="19">
@@ -4529,14 +4559,14 @@
       <c r="F57" s="19">
         <v>50</v>
       </c>
-      <c r="G57" s="30" t="s">
+      <c r="G57" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="H57" s="31"/>
-      <c r="I57" s="31"/>
-      <c r="J57" s="31"/>
-      <c r="K57" s="31"/>
-      <c r="L57" s="32"/>
+      <c r="H57" s="32"/>
+      <c r="I57" s="32"/>
+      <c r="J57" s="32"/>
+      <c r="K57" s="32"/>
+      <c r="L57" s="33"/>
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="19">
@@ -4557,12 +4587,12 @@
       <c r="F58" s="19">
         <v>50</v>
       </c>
-      <c r="G58" s="33"/>
-      <c r="H58" s="34"/>
-      <c r="I58" s="34"/>
-      <c r="J58" s="34"/>
-      <c r="K58" s="34"/>
-      <c r="L58" s="35"/>
+      <c r="G58" s="34"/>
+      <c r="H58" s="35"/>
+      <c r="I58" s="35"/>
+      <c r="J58" s="35"/>
+      <c r="K58" s="35"/>
+      <c r="L58" s="36"/>
     </row>
     <row r="59" spans="1:12">
       <c r="A59" s="19">
@@ -4583,12 +4613,12 @@
       <c r="F59" s="19">
         <v>50</v>
       </c>
-      <c r="G59" s="33"/>
-      <c r="H59" s="34"/>
-      <c r="I59" s="34"/>
-      <c r="J59" s="34"/>
-      <c r="K59" s="34"/>
-      <c r="L59" s="35"/>
+      <c r="G59" s="34"/>
+      <c r="H59" s="35"/>
+      <c r="I59" s="35"/>
+      <c r="J59" s="35"/>
+      <c r="K59" s="35"/>
+      <c r="L59" s="36"/>
     </row>
     <row r="60" spans="1:12">
       <c r="A60" s="19">
@@ -4609,12 +4639,12 @@
       <c r="F60" s="19">
         <v>50</v>
       </c>
-      <c r="G60" s="33"/>
-      <c r="H60" s="34"/>
-      <c r="I60" s="34"/>
-      <c r="J60" s="34"/>
-      <c r="K60" s="34"/>
-      <c r="L60" s="35"/>
+      <c r="G60" s="34"/>
+      <c r="H60" s="35"/>
+      <c r="I60" s="35"/>
+      <c r="J60" s="35"/>
+      <c r="K60" s="35"/>
+      <c r="L60" s="36"/>
     </row>
     <row r="61" spans="1:12">
       <c r="A61" s="19">
@@ -4635,12 +4665,12 @@
       <c r="F61" s="19">
         <v>50</v>
       </c>
-      <c r="G61" s="33"/>
-      <c r="H61" s="34"/>
-      <c r="I61" s="34"/>
-      <c r="J61" s="34"/>
-      <c r="K61" s="34"/>
-      <c r="L61" s="35"/>
+      <c r="G61" s="34"/>
+      <c r="H61" s="35"/>
+      <c r="I61" s="35"/>
+      <c r="J61" s="35"/>
+      <c r="K61" s="35"/>
+      <c r="L61" s="36"/>
     </row>
     <row r="62" spans="1:12">
       <c r="A62" s="19">
@@ -4661,12 +4691,12 @@
       <c r="F62" s="19">
         <v>50</v>
       </c>
-      <c r="G62" s="33"/>
-      <c r="H62" s="34"/>
-      <c r="I62" s="34"/>
-      <c r="J62" s="34"/>
-      <c r="K62" s="34"/>
-      <c r="L62" s="35"/>
+      <c r="G62" s="34"/>
+      <c r="H62" s="35"/>
+      <c r="I62" s="35"/>
+      <c r="J62" s="35"/>
+      <c r="K62" s="35"/>
+      <c r="L62" s="36"/>
     </row>
     <row r="63" spans="1:12">
       <c r="A63" s="22">
@@ -4687,12 +4717,12 @@
       <c r="F63" s="19">
         <v>50</v>
       </c>
-      <c r="G63" s="33"/>
-      <c r="H63" s="34"/>
-      <c r="I63" s="34"/>
-      <c r="J63" s="34"/>
-      <c r="K63" s="34"/>
-      <c r="L63" s="35"/>
+      <c r="G63" s="34"/>
+      <c r="H63" s="35"/>
+      <c r="I63" s="35"/>
+      <c r="J63" s="35"/>
+      <c r="K63" s="35"/>
+      <c r="L63" s="36"/>
     </row>
     <row r="64" spans="1:12">
       <c r="A64" s="22">
@@ -4713,12 +4743,12 @@
       <c r="F64" s="19">
         <v>50</v>
       </c>
-      <c r="G64" s="36"/>
-      <c r="H64" s="37"/>
-      <c r="I64" s="37"/>
-      <c r="J64" s="37"/>
-      <c r="K64" s="37"/>
-      <c r="L64" s="38"/>
+      <c r="G64" s="37"/>
+      <c r="H64" s="38"/>
+      <c r="I64" s="38"/>
+      <c r="J64" s="38"/>
+      <c r="K64" s="38"/>
+      <c r="L64" s="39"/>
     </row>
     <row r="65" spans="1:12">
       <c r="A65" s="22">
@@ -5117,20 +5147,20 @@
       </c>
     </row>
     <row r="76" spans="1:12" ht="30" customHeight="1">
-      <c r="A76" s="45" t="s">
+      <c r="A76" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="B76" s="45"/>
-      <c r="C76" s="45"/>
-      <c r="D76" s="45"/>
-      <c r="E76" s="45"/>
-      <c r="F76" s="45"/>
-      <c r="G76" s="45"/>
-      <c r="H76" s="45"/>
-      <c r="I76" s="45"/>
-      <c r="J76" s="45"/>
-      <c r="K76" s="45"/>
-      <c r="L76" s="45"/>
+      <c r="B76" s="30"/>
+      <c r="C76" s="30"/>
+      <c r="D76" s="30"/>
+      <c r="E76" s="30"/>
+      <c r="F76" s="30"/>
+      <c r="G76" s="30"/>
+      <c r="H76" s="30"/>
+      <c r="I76" s="30"/>
+      <c r="J76" s="30"/>
+      <c r="K76" s="30"/>
+      <c r="L76" s="30"/>
     </row>
     <row r="77" spans="1:12">
       <c r="A77" s="29" t="s">
@@ -6422,7 +6452,7 @@
     </row>
     <row r="117" spans="1:12">
       <c r="A117" s="29" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B117" s="29"/>
       <c r="C117" s="29"/>
@@ -6756,7 +6786,7 @@
     </row>
     <row r="127" spans="1:12">
       <c r="A127" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B127" s="29"/>
       <c r="C127" s="29"/>
@@ -6771,320 +6801,567 @@
       <c r="L127" s="29"/>
     </row>
     <row r="128" spans="1:12">
-      <c r="A128" s="8">
-        <v>10</v>
-      </c>
-      <c r="B128" s="9">
+      <c r="A128" s="19">
+        <v>10</v>
+      </c>
+      <c r="B128" s="20">
         <v>4991</v>
       </c>
-      <c r="C128" s="13" t="s">
+      <c r="C128" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D128" s="8">
-        <v>2500</v>
-      </c>
-      <c r="E128" s="8">
-        <v>10</v>
-      </c>
-      <c r="F128" s="8">
-        <v>50</v>
-      </c>
-      <c r="G128" s="3">
-        <v>4.6100000000000002E-2</v>
-      </c>
-      <c r="H128" s="3">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="I128" s="3">
-        <v>2.8639999999999999</v>
-      </c>
-      <c r="J128" s="3">
-        <v>62856.24</v>
-      </c>
-      <c r="K128" s="3">
-        <v>5.7270000000000001E-2</v>
-      </c>
-      <c r="L128" s="3">
-        <v>5.6890000000000003E-2</v>
-      </c>
+      <c r="D128" s="19">
+        <v>2500</v>
+      </c>
+      <c r="E128" s="19">
+        <v>10</v>
+      </c>
+      <c r="F128" s="19">
+        <v>50</v>
+      </c>
+      <c r="G128" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="H128" s="48"/>
+      <c r="I128" s="48"/>
+      <c r="J128" s="48"/>
+      <c r="K128" s="48"/>
+      <c r="L128" s="49"/>
     </row>
     <row r="129" spans="1:12">
-      <c r="A129" s="8">
-        <v>50</v>
-      </c>
-      <c r="B129" s="9">
+      <c r="A129" s="19">
+        <v>50</v>
+      </c>
+      <c r="B129" s="20">
         <v>22716</v>
       </c>
-      <c r="C129" s="13" t="s">
+      <c r="C129" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="D129" s="8">
-        <v>2500</v>
-      </c>
-      <c r="E129" s="8">
-        <v>10</v>
-      </c>
-      <c r="F129" s="8">
-        <v>50</v>
-      </c>
-      <c r="G129" s="3">
-        <v>5.2200000000000003E-2</v>
-      </c>
-      <c r="H129" s="3">
-        <v>7.6899999999999996E-2</v>
-      </c>
-      <c r="I129" s="3">
-        <v>3.1030000000000002</v>
-      </c>
-      <c r="J129" s="3">
-        <v>58004.74</v>
-      </c>
-      <c r="K129" s="3">
-        <v>6.2059999999999997E-2</v>
-      </c>
-      <c r="L129" s="3">
-        <v>6.1809999999999997E-2</v>
-      </c>
+      <c r="D129" s="19">
+        <v>2500</v>
+      </c>
+      <c r="E129" s="19">
+        <v>10</v>
+      </c>
+      <c r="F129" s="19">
+        <v>50</v>
+      </c>
+      <c r="G129" s="50"/>
+      <c r="H129" s="51"/>
+      <c r="I129" s="51"/>
+      <c r="J129" s="51"/>
+      <c r="K129" s="51"/>
+      <c r="L129" s="52"/>
     </row>
     <row r="130" spans="1:12">
-      <c r="A130" s="8">
+      <c r="A130" s="19">
         <v>100</v>
       </c>
-      <c r="B130" s="9">
+      <c r="B130" s="20">
         <v>40333</v>
       </c>
-      <c r="C130" s="13" t="s">
+      <c r="C130" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D130" s="8">
-        <v>2500</v>
-      </c>
-      <c r="E130" s="8">
-        <v>10</v>
-      </c>
-      <c r="F130" s="8">
-        <v>50</v>
-      </c>
-      <c r="G130" s="3">
-        <v>6.5799999999999997E-2</v>
-      </c>
-      <c r="H130" s="3">
-        <v>0.11020000000000001</v>
-      </c>
-      <c r="I130" s="3">
-        <v>3.8450000000000002</v>
-      </c>
-      <c r="J130" s="3">
-        <v>46809.59</v>
-      </c>
-      <c r="K130" s="3">
-        <v>7.6910000000000006E-2</v>
-      </c>
-      <c r="L130" s="3">
-        <v>7.6490000000000002E-2</v>
-      </c>
+      <c r="D130" s="19">
+        <v>2500</v>
+      </c>
+      <c r="E130" s="19">
+        <v>10</v>
+      </c>
+      <c r="F130" s="19">
+        <v>50</v>
+      </c>
+      <c r="G130" s="50"/>
+      <c r="H130" s="51"/>
+      <c r="I130" s="51"/>
+      <c r="J130" s="51"/>
+      <c r="K130" s="51"/>
+      <c r="L130" s="52"/>
     </row>
     <row r="131" spans="1:12">
-      <c r="A131" s="8">
+      <c r="A131" s="19">
         <v>250</v>
       </c>
-      <c r="B131" s="9">
+      <c r="B131" s="20">
         <v>98113</v>
       </c>
-      <c r="C131" s="13" t="s">
+      <c r="C131" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D131" s="8">
-        <v>2500</v>
-      </c>
-      <c r="E131" s="8">
-        <v>10</v>
-      </c>
-      <c r="F131" s="8">
-        <v>50</v>
-      </c>
-      <c r="G131" s="3">
-        <v>0.16</v>
-      </c>
-      <c r="H131" s="3">
-        <v>0.56169999999999998</v>
-      </c>
-      <c r="I131" s="3">
-        <v>9.4169999999999998</v>
-      </c>
-      <c r="J131" s="3">
-        <v>19115.05</v>
-      </c>
-      <c r="K131" s="3">
-        <v>0.18833</v>
-      </c>
-      <c r="L131" s="3">
-        <v>0.18359</v>
-      </c>
+      <c r="D131" s="19">
+        <v>2500</v>
+      </c>
+      <c r="E131" s="19">
+        <v>10</v>
+      </c>
+      <c r="F131" s="19">
+        <v>50</v>
+      </c>
+      <c r="G131" s="50"/>
+      <c r="H131" s="51"/>
+      <c r="I131" s="51"/>
+      <c r="J131" s="51"/>
+      <c r="K131" s="51"/>
+      <c r="L131" s="52"/>
     </row>
     <row r="132" spans="1:12">
-      <c r="A132" s="8">
+      <c r="A132" s="19">
         <v>500</v>
       </c>
-      <c r="B132" s="9">
+      <c r="B132" s="20">
         <v>191502</v>
       </c>
-      <c r="C132" s="13" t="s">
+      <c r="C132" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D132" s="8">
-        <v>2500</v>
-      </c>
-      <c r="E132" s="8">
-        <v>10</v>
-      </c>
-      <c r="F132" s="8">
-        <v>50</v>
-      </c>
-      <c r="G132" s="3">
-        <v>0.48730000000000001</v>
-      </c>
-      <c r="H132" s="3">
-        <v>1.4349000000000001</v>
-      </c>
-      <c r="I132" s="3">
-        <v>28.01</v>
-      </c>
-      <c r="J132" s="3">
-        <v>6426.31</v>
-      </c>
-      <c r="K132" s="3">
-        <v>0.56020000000000003</v>
-      </c>
-      <c r="L132" s="3">
-        <v>0.54986000000000002</v>
-      </c>
+      <c r="D132" s="19">
+        <v>2500</v>
+      </c>
+      <c r="E132" s="19">
+        <v>10</v>
+      </c>
+      <c r="F132" s="19">
+        <v>50</v>
+      </c>
+      <c r="G132" s="50"/>
+      <c r="H132" s="51"/>
+      <c r="I132" s="51"/>
+      <c r="J132" s="51"/>
+      <c r="K132" s="51"/>
+      <c r="L132" s="52"/>
     </row>
     <row r="133" spans="1:12">
-      <c r="A133" s="8">
+      <c r="A133" s="19">
         <v>1000</v>
       </c>
-      <c r="B133" s="9">
+      <c r="B133" s="20">
         <v>375114</v>
       </c>
-      <c r="C133" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D133" s="8">
-        <v>2500</v>
-      </c>
-      <c r="E133" s="8">
-        <v>10</v>
-      </c>
-      <c r="F133" s="8">
-        <v>50</v>
-      </c>
-      <c r="G133" s="3">
-        <v>1.8193999999999999</v>
-      </c>
-      <c r="H133" s="3">
-        <v>3.9373999999999998</v>
-      </c>
-      <c r="I133" s="3">
-        <v>106.005</v>
-      </c>
-      <c r="J133" s="3">
-        <v>1698.04</v>
-      </c>
-      <c r="K133" s="3">
-        <v>2.1200899999999998</v>
-      </c>
-      <c r="L133" s="3">
-        <v>2.0813299999999999</v>
-      </c>
+      <c r="C133" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D133" s="19">
+        <v>2500</v>
+      </c>
+      <c r="E133" s="19">
+        <v>10</v>
+      </c>
+      <c r="F133" s="19">
+        <v>50</v>
+      </c>
+      <c r="G133" s="50"/>
+      <c r="H133" s="51"/>
+      <c r="I133" s="51"/>
+      <c r="J133" s="51"/>
+      <c r="K133" s="51"/>
+      <c r="L133" s="52"/>
     </row>
     <row r="134" spans="1:12">
-      <c r="A134" s="5">
+      <c r="A134" s="22">
         <v>1500</v>
       </c>
-      <c r="B134" s="7">
+      <c r="B134" s="23">
         <v>550078</v>
       </c>
-      <c r="C134" s="13" t="s">
+      <c r="C134" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D134" s="5">
-        <v>2500</v>
-      </c>
-      <c r="E134" s="8">
-        <v>10</v>
-      </c>
-      <c r="F134" s="8">
-        <v>50</v>
-      </c>
-      <c r="G134" s="3"/>
-      <c r="H134" s="3"/>
-      <c r="I134" s="3"/>
-      <c r="J134" s="3"/>
-      <c r="K134" s="3"/>
-      <c r="L134" s="3"/>
+      <c r="D134" s="22">
+        <v>2500</v>
+      </c>
+      <c r="E134" s="19">
+        <v>10</v>
+      </c>
+      <c r="F134" s="19">
+        <v>50</v>
+      </c>
+      <c r="G134" s="50"/>
+      <c r="H134" s="51"/>
+      <c r="I134" s="51"/>
+      <c r="J134" s="51"/>
+      <c r="K134" s="51"/>
+      <c r="L134" s="52"/>
     </row>
     <row r="135" spans="1:12">
-      <c r="A135" s="5">
+      <c r="A135" s="22">
         <v>2000</v>
       </c>
-      <c r="B135" s="7">
+      <c r="B135" s="23">
         <v>725515</v>
       </c>
-      <c r="C135" s="13" t="s">
+      <c r="C135" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D135" s="5">
-        <v>2500</v>
-      </c>
-      <c r="E135" s="8">
-        <v>10</v>
-      </c>
-      <c r="F135" s="8">
-        <v>50</v>
-      </c>
-      <c r="G135" s="3"/>
-      <c r="H135" s="3"/>
-      <c r="I135" s="3"/>
-      <c r="J135" s="3"/>
-      <c r="K135" s="3"/>
-      <c r="L135" s="3"/>
+      <c r="D135" s="22">
+        <v>2500</v>
+      </c>
+      <c r="E135" s="19">
+        <v>10</v>
+      </c>
+      <c r="F135" s="19">
+        <v>50</v>
+      </c>
+      <c r="G135" s="50"/>
+      <c r="H135" s="51"/>
+      <c r="I135" s="51"/>
+      <c r="J135" s="51"/>
+      <c r="K135" s="51"/>
+      <c r="L135" s="52"/>
     </row>
     <row r="136" spans="1:12">
-      <c r="A136" s="5">
-        <v>2500</v>
-      </c>
-      <c r="B136" s="7">
+      <c r="A136" s="22">
+        <v>2500</v>
+      </c>
+      <c r="B136" s="23">
         <v>900517</v>
       </c>
-      <c r="C136" s="13" t="s">
+      <c r="C136" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D136" s="5">
-        <v>2500</v>
-      </c>
-      <c r="E136" s="8">
-        <v>10</v>
-      </c>
-      <c r="F136" s="8">
-        <v>50</v>
-      </c>
-      <c r="G136" s="3"/>
-      <c r="H136" s="3"/>
-      <c r="I136" s="3"/>
-      <c r="J136" s="3"/>
-      <c r="K136" s="3"/>
-      <c r="L136" s="3"/>
+      <c r="D136" s="22">
+        <v>2500</v>
+      </c>
+      <c r="E136" s="19">
+        <v>10</v>
+      </c>
+      <c r="F136" s="19">
+        <v>50</v>
+      </c>
+      <c r="G136" s="53"/>
+      <c r="H136" s="54"/>
+      <c r="I136" s="54"/>
+      <c r="J136" s="54"/>
+      <c r="K136" s="54"/>
+      <c r="L136" s="55"/>
+    </row>
+    <row r="137" spans="1:12">
+      <c r="A137" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B137" s="29"/>
+      <c r="C137" s="29"/>
+      <c r="D137" s="29"/>
+      <c r="E137" s="29"/>
+      <c r="F137" s="29"/>
+      <c r="G137" s="29"/>
+      <c r="H137" s="29"/>
+      <c r="I137" s="29"/>
+      <c r="J137" s="29"/>
+      <c r="K137" s="29"/>
+      <c r="L137" s="29"/>
+    </row>
+    <row r="138" spans="1:12">
+      <c r="A138" s="8">
+        <v>10</v>
+      </c>
+      <c r="B138" s="9">
+        <v>4991</v>
+      </c>
+      <c r="C138" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D138" s="8">
+        <v>2500</v>
+      </c>
+      <c r="E138" s="8">
+        <v>10</v>
+      </c>
+      <c r="F138" s="8">
+        <v>50</v>
+      </c>
+      <c r="G138" s="3">
+        <v>5.3199999999999997E-2</v>
+      </c>
+      <c r="H138" s="3">
+        <v>0.111</v>
+      </c>
+      <c r="I138" s="3">
+        <v>3.089</v>
+      </c>
+      <c r="J138" s="3">
+        <v>58267.39</v>
+      </c>
+      <c r="K138" s="3">
+        <v>6.1780000000000002E-2</v>
+      </c>
+      <c r="L138" s="3">
+        <v>6.114E-2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12">
+      <c r="A139" s="8">
+        <v>50</v>
+      </c>
+      <c r="B139" s="9">
+        <v>22716</v>
+      </c>
+      <c r="C139" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D139" s="8">
+        <v>2500</v>
+      </c>
+      <c r="E139" s="8">
+        <v>10</v>
+      </c>
+      <c r="F139" s="8">
+        <v>50</v>
+      </c>
+      <c r="G139" s="3">
+        <v>5.6500000000000002E-2</v>
+      </c>
+      <c r="H139" s="3">
+        <v>0.19769999999999999</v>
+      </c>
+      <c r="I139" s="3">
+        <v>3.3860000000000001</v>
+      </c>
+      <c r="J139" s="3">
+        <v>53161.69</v>
+      </c>
+      <c r="K139" s="3">
+        <v>6.7720000000000002E-2</v>
+      </c>
+      <c r="L139" s="3">
+        <v>6.6350000000000006E-2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12">
+      <c r="A140" s="8">
+        <v>100</v>
+      </c>
+      <c r="B140" s="9">
+        <v>40333</v>
+      </c>
+      <c r="C140" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D140" s="8">
+        <v>2500</v>
+      </c>
+      <c r="E140" s="8">
+        <v>10</v>
+      </c>
+      <c r="F140" s="8">
+        <v>50</v>
+      </c>
+      <c r="G140" s="3">
+        <v>7.5899999999999995E-2</v>
+      </c>
+      <c r="H140" s="3">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="I140" s="3">
+        <v>4.3369999999999997</v>
+      </c>
+      <c r="J140" s="3">
+        <v>41499.26</v>
+      </c>
+      <c r="K140" s="3">
+        <v>8.6749999999999994E-2</v>
+      </c>
+      <c r="L140" s="3">
+        <v>8.6169999999999997E-2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12">
+      <c r="A141" s="8">
+        <v>250</v>
+      </c>
+      <c r="B141" s="9">
+        <v>98113</v>
+      </c>
+      <c r="C141" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D141" s="8">
+        <v>2500</v>
+      </c>
+      <c r="E141" s="8">
+        <v>10</v>
+      </c>
+      <c r="F141" s="8">
+        <v>50</v>
+      </c>
+      <c r="G141" s="3">
+        <v>0.18720000000000001</v>
+      </c>
+      <c r="H141" s="3">
+        <v>0.34720000000000001</v>
+      </c>
+      <c r="I141" s="3">
+        <v>10.471</v>
+      </c>
+      <c r="J141" s="3">
+        <v>17191.080000000002</v>
+      </c>
+      <c r="K141" s="3">
+        <v>0.20941000000000001</v>
+      </c>
+      <c r="L141" s="3">
+        <v>0.20794000000000001</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12">
+      <c r="A142" s="8">
+        <v>500</v>
+      </c>
+      <c r="B142" s="9">
+        <v>191502</v>
+      </c>
+      <c r="C142" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D142" s="8">
+        <v>2500</v>
+      </c>
+      <c r="E142" s="8">
+        <v>10</v>
+      </c>
+      <c r="F142" s="8">
+        <v>50</v>
+      </c>
+      <c r="G142" s="3">
+        <v>0.57279999999999998</v>
+      </c>
+      <c r="H142" s="3">
+        <v>0.86209999999999998</v>
+      </c>
+      <c r="I142" s="3">
+        <v>31.501000000000001</v>
+      </c>
+      <c r="J142" s="3">
+        <v>5714.05</v>
+      </c>
+      <c r="K142" s="3">
+        <v>0.63002999999999998</v>
+      </c>
+      <c r="L142" s="3">
+        <v>0.62724999999999997</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12">
+      <c r="A143" s="8">
+        <v>1000</v>
+      </c>
+      <c r="B143" s="9">
+        <v>375114</v>
+      </c>
+      <c r="C143" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D143" s="8">
+        <v>2500</v>
+      </c>
+      <c r="E143" s="8">
+        <v>10</v>
+      </c>
+      <c r="F143" s="8">
+        <v>50</v>
+      </c>
+      <c r="G143" s="3">
+        <v>2.1537000000000002</v>
+      </c>
+      <c r="H143" s="3">
+        <v>3.7621000000000002</v>
+      </c>
+      <c r="I143" s="3">
+        <v>118.21599999999999</v>
+      </c>
+      <c r="J143" s="3">
+        <v>1522.64</v>
+      </c>
+      <c r="K143" s="3">
+        <v>2.3643200000000002</v>
+      </c>
+      <c r="L143" s="3">
+        <v>2.3531499999999999</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12">
+      <c r="A144" s="5">
+        <v>1500</v>
+      </c>
+      <c r="B144" s="7">
+        <v>550078</v>
+      </c>
+      <c r="C144" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D144" s="5">
+        <v>2500</v>
+      </c>
+      <c r="E144" s="8">
+        <v>10</v>
+      </c>
+      <c r="F144" s="8">
+        <v>50</v>
+      </c>
+      <c r="G144" s="3"/>
+      <c r="H144" s="3"/>
+      <c r="I144" s="3"/>
+      <c r="J144" s="3"/>
+      <c r="K144" s="3"/>
+      <c r="L144" s="3"/>
+    </row>
+    <row r="145" spans="1:12">
+      <c r="A145" s="5">
+        <v>2000</v>
+      </c>
+      <c r="B145" s="7">
+        <v>725515</v>
+      </c>
+      <c r="C145" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D145" s="5">
+        <v>2500</v>
+      </c>
+      <c r="E145" s="8">
+        <v>10</v>
+      </c>
+      <c r="F145" s="8">
+        <v>50</v>
+      </c>
+      <c r="G145" s="3"/>
+      <c r="H145" s="3"/>
+      <c r="I145" s="3"/>
+      <c r="J145" s="3"/>
+      <c r="K145" s="3"/>
+      <c r="L145" s="3"/>
+    </row>
+    <row r="146" spans="1:12">
+      <c r="A146" s="5">
+        <v>2500</v>
+      </c>
+      <c r="B146" s="7">
+        <v>900517</v>
+      </c>
+      <c r="C146" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D146" s="5">
+        <v>2500</v>
+      </c>
+      <c r="E146" s="8">
+        <v>10</v>
+      </c>
+      <c r="F146" s="8">
+        <v>50</v>
+      </c>
+      <c r="G146" s="3"/>
+      <c r="H146" s="3"/>
+      <c r="I146" s="3"/>
+      <c r="J146" s="3"/>
+      <c r="K146" s="3"/>
+      <c r="L146" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="A127:L127"/>
-    <mergeCell ref="A77:L77"/>
-    <mergeCell ref="A97:L97"/>
-    <mergeCell ref="A76:L76"/>
-    <mergeCell ref="A87:L87"/>
-    <mergeCell ref="A107:L107"/>
-    <mergeCell ref="A117:L117"/>
+  <mergeCells count="24">
+    <mergeCell ref="G128:L136"/>
+    <mergeCell ref="A137:L137"/>
     <mergeCell ref="A66:L66"/>
     <mergeCell ref="G57:L64"/>
     <mergeCell ref="A1:C1"/>
@@ -7100,6 +7377,13 @@
     <mergeCell ref="A36:L36"/>
     <mergeCell ref="A31:L31"/>
     <mergeCell ref="A24:L24"/>
+    <mergeCell ref="A127:L127"/>
+    <mergeCell ref="A77:L77"/>
+    <mergeCell ref="A97:L97"/>
+    <mergeCell ref="A76:L76"/>
+    <mergeCell ref="A87:L87"/>
+    <mergeCell ref="A107:L107"/>
+    <mergeCell ref="A117:L117"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7130,11 +7414,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
       <c r="D1" s="24"/>
       <c r="E1" s="24"/>
     </row>
@@ -7145,28 +7429,28 @@
       <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:14" ht="15.75">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
       <c r="D3" s="46" t="s">
         <v>44</v>
       </c>
       <c r="E3" s="47"/>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43" t="s">
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="6" t="s">
@@ -7616,11 +7900,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
       <c r="D1" s="26"/>
       <c r="E1" s="26"/>
     </row>
@@ -7631,28 +7915,28 @@
       <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:14" ht="15.75">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
       <c r="D3" s="46" t="s">
         <v>44</v>
       </c>
       <c r="E3" s="47"/>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43" t="s">
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="6" t="s">
@@ -8021,11 +8305,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
       <c r="D1" s="25"/>
       <c r="E1" s="25"/>
     </row>
@@ -8036,28 +8320,28 @@
       <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:14" ht="15.75">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
       <c r="D3" s="46" t="s">
         <v>44</v>
       </c>
       <c r="E3" s="47"/>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43" t="s">
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="6" t="s">

</xml_diff>

<commit_message>
More work on the new RDFa 1.1 Core parser, still lots of bugs to be ironed out atm
</commit_message>
<xml_diff>
--- a/Benchmarks/dotNetRDF BSBM Benchmark.xlsx
+++ b/Benchmarks/dotNetRDF BSBM Benchmark.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="62">
   <si>
     <t>BSBM Benchmarks</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>Leviathan Engine - Version 0.4.2 (With Identity Filter optimisation enabled) using Default Optimiser</t>
+  </si>
+  <si>
+    <t>Leviathan Engine - Version 0.4.2 (With improved internal data structures) using Default Optimiser</t>
   </si>
 </sst>
 </file>
@@ -492,14 +495,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -543,35 +567,14 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1163,11 +1166,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="93539712"/>
-        <c:axId val="93549696"/>
+        <c:axId val="81735040"/>
+        <c:axId val="81745024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="93539712"/>
+        <c:axId val="81735040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1175,14 +1178,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93549696"/>
+        <c:crossAx val="81745024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93549696"/>
+        <c:axId val="81745024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1208,7 +1211,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93539712"/>
+        <c:crossAx val="81735040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1220,7 +1223,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1558,11 +1561,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="93722112"/>
-        <c:axId val="93723648"/>
+        <c:axId val="81782272"/>
+        <c:axId val="81783808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="93722112"/>
+        <c:axId val="81782272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1570,14 +1573,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93723648"/>
+        <c:crossAx val="81783808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93723648"/>
+        <c:axId val="81783808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1603,7 +1606,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93722112"/>
+        <c:crossAx val="81782272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1615,7 +1618,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1821,25 +1824,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="93769728"/>
-        <c:axId val="93771264"/>
+        <c:axId val="81965056"/>
+        <c:axId val="81966592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="93769728"/>
+        <c:axId val="81965056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93771264"/>
+        <c:crossAx val="81966592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93771264"/>
+        <c:axId val="81966592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1864,7 +1867,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93769728"/>
+        <c:crossAx val="81965056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1876,7 +1879,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2208,25 +2211,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="97010048"/>
-        <c:axId val="97011584"/>
+        <c:axId val="82125184"/>
+        <c:axId val="82126720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="97010048"/>
+        <c:axId val="82125184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97011584"/>
+        <c:crossAx val="82126720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97011584"/>
+        <c:axId val="82126720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2251,7 +2254,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97010048"/>
+        <c:crossAx val="82125184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2263,7 +2266,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2684,11 +2687,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L146"/>
+  <dimension ref="A1:L156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A137" sqref="A137:L137"/>
+      <pane ySplit="4" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G154" sqref="G154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2707,34 +2710,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1">
       <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="15.75">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44" t="s">
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44" t="s">
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="6" t="s">
@@ -2775,20 +2778,20 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="43"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="50"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="5">
@@ -2867,20 +2870,20 @@
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="43"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="50"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="8">
@@ -3035,20 +3038,20 @@
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="42"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="42"/>
-      <c r="K13" s="42"/>
-      <c r="L13" s="43"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="49"/>
+      <c r="L13" s="50"/>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="5">
@@ -3279,20 +3282,20 @@
       </c>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="42"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="42"/>
-      <c r="L20" s="43"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="50"/>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="8">
@@ -3409,20 +3412,20 @@
       </c>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="42"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
-      <c r="K24" s="42"/>
-      <c r="L24" s="43"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="49"/>
+      <c r="L24" s="50"/>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="8">
@@ -3653,20 +3656,20 @@
       </c>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="41" t="s">
+      <c r="A31" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="42"/>
-      <c r="C31" s="42"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="42"/>
-      <c r="J31" s="42"/>
-      <c r="K31" s="42"/>
-      <c r="L31" s="43"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="49"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="49"/>
+      <c r="J31" s="49"/>
+      <c r="K31" s="49"/>
+      <c r="L31" s="50"/>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="8">
@@ -3821,20 +3824,20 @@
       </c>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="41" t="s">
+      <c r="A36" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="42"/>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="42"/>
-      <c r="G36" s="42"/>
-      <c r="H36" s="42"/>
-      <c r="I36" s="42"/>
-      <c r="J36" s="42"/>
-      <c r="K36" s="42"/>
-      <c r="L36" s="43"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="49"/>
+      <c r="J36" s="49"/>
+      <c r="K36" s="49"/>
+      <c r="L36" s="50"/>
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="8">
@@ -4141,20 +4144,20 @@
       </c>
     </row>
     <row r="45" spans="1:12">
-      <c r="A45" s="29" t="s">
+      <c r="A45" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="29"/>
-      <c r="G45" s="29"/>
-      <c r="H45" s="29"/>
-      <c r="I45" s="29"/>
-      <c r="J45" s="29"/>
-      <c r="K45" s="29"/>
-      <c r="L45" s="29"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="38"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="38"/>
+      <c r="F45" s="38"/>
+      <c r="G45" s="38"/>
+      <c r="H45" s="38"/>
+      <c r="I45" s="38"/>
+      <c r="J45" s="38"/>
+      <c r="K45" s="38"/>
+      <c r="L45" s="38"/>
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="8">
@@ -4525,20 +4528,20 @@
       <c r="L55" s="8"/>
     </row>
     <row r="56" spans="1:12">
-      <c r="A56" s="45" t="s">
+      <c r="A56" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="B56" s="45"/>
-      <c r="C56" s="45"/>
-      <c r="D56" s="45"/>
-      <c r="E56" s="45"/>
-      <c r="F56" s="45"/>
-      <c r="G56" s="45"/>
-      <c r="H56" s="45"/>
-      <c r="I56" s="45"/>
-      <c r="J56" s="45"/>
-      <c r="K56" s="45"/>
-      <c r="L56" s="45"/>
+      <c r="B56" s="52"/>
+      <c r="C56" s="52"/>
+      <c r="D56" s="52"/>
+      <c r="E56" s="52"/>
+      <c r="F56" s="52"/>
+      <c r="G56" s="52"/>
+      <c r="H56" s="52"/>
+      <c r="I56" s="52"/>
+      <c r="J56" s="52"/>
+      <c r="K56" s="52"/>
+      <c r="L56" s="52"/>
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="19">
@@ -4559,14 +4562,14 @@
       <c r="F57" s="19">
         <v>50</v>
       </c>
-      <c r="G57" s="31" t="s">
+      <c r="G57" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="H57" s="32"/>
-      <c r="I57" s="32"/>
-      <c r="J57" s="32"/>
-      <c r="K57" s="32"/>
-      <c r="L57" s="33"/>
+      <c r="H57" s="39"/>
+      <c r="I57" s="39"/>
+      <c r="J57" s="39"/>
+      <c r="K57" s="39"/>
+      <c r="L57" s="40"/>
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="19">
@@ -4587,12 +4590,12 @@
       <c r="F58" s="19">
         <v>50</v>
       </c>
-      <c r="G58" s="34"/>
-      <c r="H58" s="35"/>
-      <c r="I58" s="35"/>
-      <c r="J58" s="35"/>
-      <c r="K58" s="35"/>
-      <c r="L58" s="36"/>
+      <c r="G58" s="41"/>
+      <c r="H58" s="42"/>
+      <c r="I58" s="42"/>
+      <c r="J58" s="42"/>
+      <c r="K58" s="42"/>
+      <c r="L58" s="43"/>
     </row>
     <row r="59" spans="1:12">
       <c r="A59" s="19">
@@ -4613,12 +4616,12 @@
       <c r="F59" s="19">
         <v>50</v>
       </c>
-      <c r="G59" s="34"/>
-      <c r="H59" s="35"/>
-      <c r="I59" s="35"/>
-      <c r="J59" s="35"/>
-      <c r="K59" s="35"/>
-      <c r="L59" s="36"/>
+      <c r="G59" s="41"/>
+      <c r="H59" s="42"/>
+      <c r="I59" s="42"/>
+      <c r="J59" s="42"/>
+      <c r="K59" s="42"/>
+      <c r="L59" s="43"/>
     </row>
     <row r="60" spans="1:12">
       <c r="A60" s="19">
@@ -4639,12 +4642,12 @@
       <c r="F60" s="19">
         <v>50</v>
       </c>
-      <c r="G60" s="34"/>
-      <c r="H60" s="35"/>
-      <c r="I60" s="35"/>
-      <c r="J60" s="35"/>
-      <c r="K60" s="35"/>
-      <c r="L60" s="36"/>
+      <c r="G60" s="41"/>
+      <c r="H60" s="42"/>
+      <c r="I60" s="42"/>
+      <c r="J60" s="42"/>
+      <c r="K60" s="42"/>
+      <c r="L60" s="43"/>
     </row>
     <row r="61" spans="1:12">
       <c r="A61" s="19">
@@ -4665,12 +4668,12 @@
       <c r="F61" s="19">
         <v>50</v>
       </c>
-      <c r="G61" s="34"/>
-      <c r="H61" s="35"/>
-      <c r="I61" s="35"/>
-      <c r="J61" s="35"/>
-      <c r="K61" s="35"/>
-      <c r="L61" s="36"/>
+      <c r="G61" s="41"/>
+      <c r="H61" s="42"/>
+      <c r="I61" s="42"/>
+      <c r="J61" s="42"/>
+      <c r="K61" s="42"/>
+      <c r="L61" s="43"/>
     </row>
     <row r="62" spans="1:12">
       <c r="A62" s="19">
@@ -4691,12 +4694,12 @@
       <c r="F62" s="19">
         <v>50</v>
       </c>
-      <c r="G62" s="34"/>
-      <c r="H62" s="35"/>
-      <c r="I62" s="35"/>
-      <c r="J62" s="35"/>
-      <c r="K62" s="35"/>
-      <c r="L62" s="36"/>
+      <c r="G62" s="41"/>
+      <c r="H62" s="42"/>
+      <c r="I62" s="42"/>
+      <c r="J62" s="42"/>
+      <c r="K62" s="42"/>
+      <c r="L62" s="43"/>
     </row>
     <row r="63" spans="1:12">
       <c r="A63" s="22">
@@ -4717,12 +4720,12 @@
       <c r="F63" s="19">
         <v>50</v>
       </c>
-      <c r="G63" s="34"/>
-      <c r="H63" s="35"/>
-      <c r="I63" s="35"/>
-      <c r="J63" s="35"/>
-      <c r="K63" s="35"/>
-      <c r="L63" s="36"/>
+      <c r="G63" s="41"/>
+      <c r="H63" s="42"/>
+      <c r="I63" s="42"/>
+      <c r="J63" s="42"/>
+      <c r="K63" s="42"/>
+      <c r="L63" s="43"/>
     </row>
     <row r="64" spans="1:12">
       <c r="A64" s="22">
@@ -4743,12 +4746,12 @@
       <c r="F64" s="19">
         <v>50</v>
       </c>
-      <c r="G64" s="37"/>
-      <c r="H64" s="38"/>
-      <c r="I64" s="38"/>
-      <c r="J64" s="38"/>
-      <c r="K64" s="38"/>
-      <c r="L64" s="39"/>
+      <c r="G64" s="44"/>
+      <c r="H64" s="45"/>
+      <c r="I64" s="45"/>
+      <c r="J64" s="45"/>
+      <c r="K64" s="45"/>
+      <c r="L64" s="46"/>
     </row>
     <row r="65" spans="1:12">
       <c r="A65" s="22">
@@ -4789,20 +4792,20 @@
       </c>
     </row>
     <row r="66" spans="1:12">
-      <c r="A66" s="29" t="s">
+      <c r="A66" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="B66" s="29"/>
-      <c r="C66" s="29"/>
-      <c r="D66" s="29"/>
-      <c r="E66" s="29"/>
-      <c r="F66" s="29"/>
-      <c r="G66" s="29"/>
-      <c r="H66" s="29"/>
-      <c r="I66" s="29"/>
-      <c r="J66" s="29"/>
-      <c r="K66" s="29"/>
-      <c r="L66" s="29"/>
+      <c r="B66" s="38"/>
+      <c r="C66" s="38"/>
+      <c r="D66" s="38"/>
+      <c r="E66" s="38"/>
+      <c r="F66" s="38"/>
+      <c r="G66" s="38"/>
+      <c r="H66" s="38"/>
+      <c r="I66" s="38"/>
+      <c r="J66" s="38"/>
+      <c r="K66" s="38"/>
+      <c r="L66" s="38"/>
     </row>
     <row r="67" spans="1:12">
       <c r="A67" s="8">
@@ -5147,36 +5150,36 @@
       </c>
     </row>
     <row r="76" spans="1:12" ht="30" customHeight="1">
-      <c r="A76" s="30" t="s">
+      <c r="A76" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="B76" s="30"/>
-      <c r="C76" s="30"/>
-      <c r="D76" s="30"/>
-      <c r="E76" s="30"/>
-      <c r="F76" s="30"/>
-      <c r="G76" s="30"/>
-      <c r="H76" s="30"/>
-      <c r="I76" s="30"/>
-      <c r="J76" s="30"/>
-      <c r="K76" s="30"/>
-      <c r="L76" s="30"/>
+      <c r="B76" s="53"/>
+      <c r="C76" s="53"/>
+      <c r="D76" s="53"/>
+      <c r="E76" s="53"/>
+      <c r="F76" s="53"/>
+      <c r="G76" s="53"/>
+      <c r="H76" s="53"/>
+      <c r="I76" s="53"/>
+      <c r="J76" s="53"/>
+      <c r="K76" s="53"/>
+      <c r="L76" s="53"/>
     </row>
     <row r="77" spans="1:12">
-      <c r="A77" s="29" t="s">
+      <c r="A77" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="B77" s="29"/>
-      <c r="C77" s="29"/>
-      <c r="D77" s="29"/>
-      <c r="E77" s="29"/>
-      <c r="F77" s="29"/>
-      <c r="G77" s="29"/>
-      <c r="H77" s="29"/>
-      <c r="I77" s="29"/>
-      <c r="J77" s="29"/>
-      <c r="K77" s="29"/>
-      <c r="L77" s="29"/>
+      <c r="B77" s="38"/>
+      <c r="C77" s="38"/>
+      <c r="D77" s="38"/>
+      <c r="E77" s="38"/>
+      <c r="F77" s="38"/>
+      <c r="G77" s="38"/>
+      <c r="H77" s="38"/>
+      <c r="I77" s="38"/>
+      <c r="J77" s="38"/>
+      <c r="K77" s="38"/>
+      <c r="L77" s="38"/>
     </row>
     <row r="78" spans="1:12">
       <c r="A78" s="8">
@@ -5497,20 +5500,20 @@
       <c r="L86" s="8"/>
     </row>
     <row r="87" spans="1:12">
-      <c r="A87" s="29" t="s">
+      <c r="A87" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="B87" s="29"/>
-      <c r="C87" s="29"/>
-      <c r="D87" s="29"/>
-      <c r="E87" s="29"/>
-      <c r="F87" s="29"/>
-      <c r="G87" s="29"/>
-      <c r="H87" s="29"/>
-      <c r="I87" s="29"/>
-      <c r="J87" s="29"/>
-      <c r="K87" s="29"/>
-      <c r="L87" s="29"/>
+      <c r="B87" s="38"/>
+      <c r="C87" s="38"/>
+      <c r="D87" s="38"/>
+      <c r="E87" s="38"/>
+      <c r="F87" s="38"/>
+      <c r="G87" s="38"/>
+      <c r="H87" s="38"/>
+      <c r="I87" s="38"/>
+      <c r="J87" s="38"/>
+      <c r="K87" s="38"/>
+      <c r="L87" s="38"/>
     </row>
     <row r="88" spans="1:12">
       <c r="A88" s="8">
@@ -5807,20 +5810,20 @@
       <c r="L96" s="8"/>
     </row>
     <row r="97" spans="1:12">
-      <c r="A97" s="29" t="s">
+      <c r="A97" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="B97" s="29"/>
-      <c r="C97" s="29"/>
-      <c r="D97" s="29"/>
-      <c r="E97" s="29"/>
-      <c r="F97" s="29"/>
-      <c r="G97" s="29"/>
-      <c r="H97" s="29"/>
-      <c r="I97" s="29"/>
-      <c r="J97" s="29"/>
-      <c r="K97" s="29"/>
-      <c r="L97" s="29"/>
+      <c r="B97" s="38"/>
+      <c r="C97" s="38"/>
+      <c r="D97" s="38"/>
+      <c r="E97" s="38"/>
+      <c r="F97" s="38"/>
+      <c r="G97" s="38"/>
+      <c r="H97" s="38"/>
+      <c r="I97" s="38"/>
+      <c r="J97" s="38"/>
+      <c r="K97" s="38"/>
+      <c r="L97" s="38"/>
     </row>
     <row r="98" spans="1:12">
       <c r="A98" s="8">
@@ -6141,20 +6144,20 @@
       <c r="L106" s="8"/>
     </row>
     <row r="107" spans="1:12">
-      <c r="A107" s="29" t="s">
+      <c r="A107" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="B107" s="29"/>
-      <c r="C107" s="29"/>
-      <c r="D107" s="29"/>
-      <c r="E107" s="29"/>
-      <c r="F107" s="29"/>
-      <c r="G107" s="29"/>
-      <c r="H107" s="29"/>
-      <c r="I107" s="29"/>
-      <c r="J107" s="29"/>
-      <c r="K107" s="29"/>
-      <c r="L107" s="29"/>
+      <c r="B107" s="38"/>
+      <c r="C107" s="38"/>
+      <c r="D107" s="38"/>
+      <c r="E107" s="38"/>
+      <c r="F107" s="38"/>
+      <c r="G107" s="38"/>
+      <c r="H107" s="38"/>
+      <c r="I107" s="38"/>
+      <c r="J107" s="38"/>
+      <c r="K107" s="38"/>
+      <c r="L107" s="38"/>
     </row>
     <row r="108" spans="1:12">
       <c r="A108" s="8">
@@ -6451,20 +6454,20 @@
       <c r="L116" s="8"/>
     </row>
     <row r="117" spans="1:12">
-      <c r="A117" s="29" t="s">
+      <c r="A117" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="B117" s="29"/>
-      <c r="C117" s="29"/>
-      <c r="D117" s="29"/>
-      <c r="E117" s="29"/>
-      <c r="F117" s="29"/>
-      <c r="G117" s="29"/>
-      <c r="H117" s="29"/>
-      <c r="I117" s="29"/>
-      <c r="J117" s="29"/>
-      <c r="K117" s="29"/>
-      <c r="L117" s="29"/>
+      <c r="B117" s="38"/>
+      <c r="C117" s="38"/>
+      <c r="D117" s="38"/>
+      <c r="E117" s="38"/>
+      <c r="F117" s="38"/>
+      <c r="G117" s="38"/>
+      <c r="H117" s="38"/>
+      <c r="I117" s="38"/>
+      <c r="J117" s="38"/>
+      <c r="K117" s="38"/>
+      <c r="L117" s="38"/>
     </row>
     <row r="118" spans="1:12">
       <c r="A118" s="8">
@@ -6785,20 +6788,20 @@
       <c r="L126" s="3"/>
     </row>
     <row r="127" spans="1:12">
-      <c r="A127" s="29" t="s">
+      <c r="A127" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="B127" s="29"/>
-      <c r="C127" s="29"/>
-      <c r="D127" s="29"/>
-      <c r="E127" s="29"/>
-      <c r="F127" s="29"/>
-      <c r="G127" s="29"/>
-      <c r="H127" s="29"/>
-      <c r="I127" s="29"/>
-      <c r="J127" s="29"/>
-      <c r="K127" s="29"/>
-      <c r="L127" s="29"/>
+      <c r="B127" s="38"/>
+      <c r="C127" s="38"/>
+      <c r="D127" s="38"/>
+      <c r="E127" s="38"/>
+      <c r="F127" s="38"/>
+      <c r="G127" s="38"/>
+      <c r="H127" s="38"/>
+      <c r="I127" s="38"/>
+      <c r="J127" s="38"/>
+      <c r="K127" s="38"/>
+      <c r="L127" s="38"/>
     </row>
     <row r="128" spans="1:12">
       <c r="A128" s="19">
@@ -6819,14 +6822,14 @@
       <c r="F128" s="19">
         <v>50</v>
       </c>
-      <c r="G128" s="31" t="s">
+      <c r="G128" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="H128" s="48"/>
-      <c r="I128" s="48"/>
-      <c r="J128" s="48"/>
-      <c r="K128" s="48"/>
-      <c r="L128" s="49"/>
+      <c r="H128" s="30"/>
+      <c r="I128" s="30"/>
+      <c r="J128" s="30"/>
+      <c r="K128" s="30"/>
+      <c r="L128" s="31"/>
     </row>
     <row r="129" spans="1:12">
       <c r="A129" s="19">
@@ -6847,12 +6850,12 @@
       <c r="F129" s="19">
         <v>50</v>
       </c>
-      <c r="G129" s="50"/>
-      <c r="H129" s="51"/>
-      <c r="I129" s="51"/>
-      <c r="J129" s="51"/>
-      <c r="K129" s="51"/>
-      <c r="L129" s="52"/>
+      <c r="G129" s="32"/>
+      <c r="H129" s="33"/>
+      <c r="I129" s="33"/>
+      <c r="J129" s="33"/>
+      <c r="K129" s="33"/>
+      <c r="L129" s="34"/>
     </row>
     <row r="130" spans="1:12">
       <c r="A130" s="19">
@@ -6873,12 +6876,12 @@
       <c r="F130" s="19">
         <v>50</v>
       </c>
-      <c r="G130" s="50"/>
-      <c r="H130" s="51"/>
-      <c r="I130" s="51"/>
-      <c r="J130" s="51"/>
-      <c r="K130" s="51"/>
-      <c r="L130" s="52"/>
+      <c r="G130" s="32"/>
+      <c r="H130" s="33"/>
+      <c r="I130" s="33"/>
+      <c r="J130" s="33"/>
+      <c r="K130" s="33"/>
+      <c r="L130" s="34"/>
     </row>
     <row r="131" spans="1:12">
       <c r="A131" s="19">
@@ -6899,12 +6902,12 @@
       <c r="F131" s="19">
         <v>50</v>
       </c>
-      <c r="G131" s="50"/>
-      <c r="H131" s="51"/>
-      <c r="I131" s="51"/>
-      <c r="J131" s="51"/>
-      <c r="K131" s="51"/>
-      <c r="L131" s="52"/>
+      <c r="G131" s="32"/>
+      <c r="H131" s="33"/>
+      <c r="I131" s="33"/>
+      <c r="J131" s="33"/>
+      <c r="K131" s="33"/>
+      <c r="L131" s="34"/>
     </row>
     <row r="132" spans="1:12">
       <c r="A132" s="19">
@@ -6925,12 +6928,12 @@
       <c r="F132" s="19">
         <v>50</v>
       </c>
-      <c r="G132" s="50"/>
-      <c r="H132" s="51"/>
-      <c r="I132" s="51"/>
-      <c r="J132" s="51"/>
-      <c r="K132" s="51"/>
-      <c r="L132" s="52"/>
+      <c r="G132" s="32"/>
+      <c r="H132" s="33"/>
+      <c r="I132" s="33"/>
+      <c r="J132" s="33"/>
+      <c r="K132" s="33"/>
+      <c r="L132" s="34"/>
     </row>
     <row r="133" spans="1:12">
       <c r="A133" s="19">
@@ -6951,12 +6954,12 @@
       <c r="F133" s="19">
         <v>50</v>
       </c>
-      <c r="G133" s="50"/>
-      <c r="H133" s="51"/>
-      <c r="I133" s="51"/>
-      <c r="J133" s="51"/>
-      <c r="K133" s="51"/>
-      <c r="L133" s="52"/>
+      <c r="G133" s="32"/>
+      <c r="H133" s="33"/>
+      <c r="I133" s="33"/>
+      <c r="J133" s="33"/>
+      <c r="K133" s="33"/>
+      <c r="L133" s="34"/>
     </row>
     <row r="134" spans="1:12">
       <c r="A134" s="22">
@@ -6977,12 +6980,12 @@
       <c r="F134" s="19">
         <v>50</v>
       </c>
-      <c r="G134" s="50"/>
-      <c r="H134" s="51"/>
-      <c r="I134" s="51"/>
-      <c r="J134" s="51"/>
-      <c r="K134" s="51"/>
-      <c r="L134" s="52"/>
+      <c r="G134" s="32"/>
+      <c r="H134" s="33"/>
+      <c r="I134" s="33"/>
+      <c r="J134" s="33"/>
+      <c r="K134" s="33"/>
+      <c r="L134" s="34"/>
     </row>
     <row r="135" spans="1:12">
       <c r="A135" s="22">
@@ -7003,12 +7006,12 @@
       <c r="F135" s="19">
         <v>50</v>
       </c>
-      <c r="G135" s="50"/>
-      <c r="H135" s="51"/>
-      <c r="I135" s="51"/>
-      <c r="J135" s="51"/>
-      <c r="K135" s="51"/>
-      <c r="L135" s="52"/>
+      <c r="G135" s="32"/>
+      <c r="H135" s="33"/>
+      <c r="I135" s="33"/>
+      <c r="J135" s="33"/>
+      <c r="K135" s="33"/>
+      <c r="L135" s="34"/>
     </row>
     <row r="136" spans="1:12">
       <c r="A136" s="22">
@@ -7029,28 +7032,28 @@
       <c r="F136" s="19">
         <v>50</v>
       </c>
-      <c r="G136" s="53"/>
-      <c r="H136" s="54"/>
-      <c r="I136" s="54"/>
-      <c r="J136" s="54"/>
-      <c r="K136" s="54"/>
-      <c r="L136" s="55"/>
+      <c r="G136" s="35"/>
+      <c r="H136" s="36"/>
+      <c r="I136" s="36"/>
+      <c r="J136" s="36"/>
+      <c r="K136" s="36"/>
+      <c r="L136" s="37"/>
     </row>
     <row r="137" spans="1:12">
-      <c r="A137" s="29" t="s">
+      <c r="A137" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="B137" s="29"/>
-      <c r="C137" s="29"/>
-      <c r="D137" s="29"/>
-      <c r="E137" s="29"/>
-      <c r="F137" s="29"/>
-      <c r="G137" s="29"/>
-      <c r="H137" s="29"/>
-      <c r="I137" s="29"/>
-      <c r="J137" s="29"/>
-      <c r="K137" s="29"/>
-      <c r="L137" s="29"/>
+      <c r="B137" s="38"/>
+      <c r="C137" s="38"/>
+      <c r="D137" s="38"/>
+      <c r="E137" s="38"/>
+      <c r="F137" s="38"/>
+      <c r="G137" s="38"/>
+      <c r="H137" s="38"/>
+      <c r="I137" s="38"/>
+      <c r="J137" s="38"/>
+      <c r="K137" s="38"/>
+      <c r="L137" s="38"/>
     </row>
     <row r="138" spans="1:12">
       <c r="A138" s="8">
@@ -7358,8 +7361,339 @@
       <c r="K146" s="3"/>
       <c r="L146" s="3"/>
     </row>
+    <row r="147" spans="1:12">
+      <c r="A147" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="B147" s="38"/>
+      <c r="C147" s="38"/>
+      <c r="D147" s="38"/>
+      <c r="E147" s="38"/>
+      <c r="F147" s="38"/>
+      <c r="G147" s="38"/>
+      <c r="H147" s="38"/>
+      <c r="I147" s="38"/>
+      <c r="J147" s="38"/>
+      <c r="K147" s="38"/>
+      <c r="L147" s="38"/>
+    </row>
+    <row r="148" spans="1:12">
+      <c r="A148" s="8">
+        <v>10</v>
+      </c>
+      <c r="B148" s="9">
+        <v>4991</v>
+      </c>
+      <c r="C148" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D148" s="8">
+        <v>2500</v>
+      </c>
+      <c r="E148" s="8">
+        <v>10</v>
+      </c>
+      <c r="F148" s="8">
+        <v>50</v>
+      </c>
+      <c r="G148" s="3">
+        <v>4.7699999999999999E-2</v>
+      </c>
+      <c r="H148" s="3">
+        <v>0.10829999999999999</v>
+      </c>
+      <c r="I148" s="3">
+        <v>3.0680000000000001</v>
+      </c>
+      <c r="J148" s="3">
+        <v>58674.09</v>
+      </c>
+      <c r="K148" s="3">
+        <v>6.1359999999999998E-2</v>
+      </c>
+      <c r="L148" s="3">
+        <v>6.0400000000000002E-2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12">
+      <c r="A149" s="8">
+        <v>50</v>
+      </c>
+      <c r="B149" s="9">
+        <v>22716</v>
+      </c>
+      <c r="C149" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D149" s="8">
+        <v>2500</v>
+      </c>
+      <c r="E149" s="8">
+        <v>10</v>
+      </c>
+      <c r="F149" s="8">
+        <v>50</v>
+      </c>
+      <c r="G149" s="3">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="H149" s="3">
+        <v>0.1183</v>
+      </c>
+      <c r="I149" s="3">
+        <v>3.1989999999999998</v>
+      </c>
+      <c r="J149" s="3">
+        <v>56265.8</v>
+      </c>
+      <c r="K149" s="3">
+        <v>6.3979999999999995E-2</v>
+      </c>
+      <c r="L149" s="3">
+        <v>6.3299999999999995E-2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12">
+      <c r="A150" s="8">
+        <v>100</v>
+      </c>
+      <c r="B150" s="9">
+        <v>40333</v>
+      </c>
+      <c r="C150" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D150" s="8">
+        <v>2500</v>
+      </c>
+      <c r="E150" s="8">
+        <v>10</v>
+      </c>
+      <c r="F150" s="8">
+        <v>50</v>
+      </c>
+      <c r="G150" s="3">
+        <v>7.1099999999999997E-2</v>
+      </c>
+      <c r="H150" s="3">
+        <v>0.1192</v>
+      </c>
+      <c r="I150" s="3">
+        <v>4.1239999999999997</v>
+      </c>
+      <c r="J150" s="3">
+        <v>43646.77</v>
+      </c>
+      <c r="K150" s="3">
+        <v>8.2479999999999998E-2</v>
+      </c>
+      <c r="L150" s="3">
+        <v>8.1989999999999993E-2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12">
+      <c r="A151" s="8">
+        <v>250</v>
+      </c>
+      <c r="B151" s="9">
+        <v>98113</v>
+      </c>
+      <c r="C151" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D151" s="8">
+        <v>2500</v>
+      </c>
+      <c r="E151" s="8">
+        <v>10</v>
+      </c>
+      <c r="F151" s="8">
+        <v>50</v>
+      </c>
+      <c r="G151" s="3">
+        <v>0.18160000000000001</v>
+      </c>
+      <c r="H151" s="3">
+        <v>0.32479999999999998</v>
+      </c>
+      <c r="I151" s="3">
+        <v>10.210000000000001</v>
+      </c>
+      <c r="J151" s="3">
+        <v>17629.28</v>
+      </c>
+      <c r="K151" s="3">
+        <v>0.20421</v>
+      </c>
+      <c r="L151" s="3">
+        <v>0.20244999999999999</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12">
+      <c r="A152" s="8">
+        <v>500</v>
+      </c>
+      <c r="B152" s="9">
+        <v>191502</v>
+      </c>
+      <c r="C152" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D152" s="8">
+        <v>2500</v>
+      </c>
+      <c r="E152" s="8">
+        <v>10</v>
+      </c>
+      <c r="F152" s="8">
+        <v>50</v>
+      </c>
+      <c r="G152" s="3">
+        <v>0.57030000000000003</v>
+      </c>
+      <c r="H152" s="3">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="I152" s="3">
+        <v>31.277999999999999</v>
+      </c>
+      <c r="J152" s="3">
+        <v>5754.84</v>
+      </c>
+      <c r="K152" s="3">
+        <v>0.63556000000000001</v>
+      </c>
+      <c r="L152" s="3">
+        <v>0.62250000000000005</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12">
+      <c r="A153" s="8">
+        <v>1000</v>
+      </c>
+      <c r="B153" s="9">
+        <v>375114</v>
+      </c>
+      <c r="C153" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D153" s="8">
+        <v>2500</v>
+      </c>
+      <c r="E153" s="8">
+        <v>10</v>
+      </c>
+      <c r="F153" s="8">
+        <v>50</v>
+      </c>
+      <c r="G153" s="3">
+        <v>2.2107999999999999</v>
+      </c>
+      <c r="H153" s="3">
+        <v>2.9741</v>
+      </c>
+      <c r="I153" s="3">
+        <v>119.45099999999999</v>
+      </c>
+      <c r="J153" s="3">
+        <v>1506.9</v>
+      </c>
+      <c r="K153" s="3">
+        <v>2.3890099999999999</v>
+      </c>
+      <c r="L153" s="3">
+        <v>2.3825500000000002</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12">
+      <c r="A154" s="5">
+        <v>1500</v>
+      </c>
+      <c r="B154" s="7">
+        <v>550078</v>
+      </c>
+      <c r="C154" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D154" s="5">
+        <v>2500</v>
+      </c>
+      <c r="E154" s="8">
+        <v>10</v>
+      </c>
+      <c r="F154" s="8">
+        <v>50</v>
+      </c>
+      <c r="G154" s="3"/>
+      <c r="H154" s="3"/>
+      <c r="I154" s="3"/>
+      <c r="J154" s="3"/>
+      <c r="K154" s="3"/>
+      <c r="L154" s="3"/>
+    </row>
+    <row r="155" spans="1:12">
+      <c r="A155" s="5">
+        <v>2000</v>
+      </c>
+      <c r="B155" s="7">
+        <v>725515</v>
+      </c>
+      <c r="C155" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D155" s="5">
+        <v>2500</v>
+      </c>
+      <c r="E155" s="8">
+        <v>10</v>
+      </c>
+      <c r="F155" s="8">
+        <v>50</v>
+      </c>
+      <c r="G155" s="3"/>
+      <c r="H155" s="3"/>
+      <c r="I155" s="3"/>
+      <c r="J155" s="3"/>
+      <c r="K155" s="3"/>
+      <c r="L155" s="3"/>
+    </row>
+    <row r="156" spans="1:12">
+      <c r="A156" s="5">
+        <v>2500</v>
+      </c>
+      <c r="B156" s="7">
+        <v>900517</v>
+      </c>
+      <c r="C156" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D156" s="5">
+        <v>2500</v>
+      </c>
+      <c r="E156" s="8">
+        <v>10</v>
+      </c>
+      <c r="F156" s="8">
+        <v>50</v>
+      </c>
+      <c r="G156" s="3"/>
+      <c r="H156" s="3"/>
+      <c r="I156" s="3"/>
+      <c r="J156" s="3"/>
+      <c r="K156" s="3"/>
+      <c r="L156" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="25">
+    <mergeCell ref="A147:L147"/>
+    <mergeCell ref="A24:L24"/>
+    <mergeCell ref="A127:L127"/>
+    <mergeCell ref="A77:L77"/>
+    <mergeCell ref="A97:L97"/>
+    <mergeCell ref="A76:L76"/>
+    <mergeCell ref="A87:L87"/>
+    <mergeCell ref="A107:L107"/>
+    <mergeCell ref="A117:L117"/>
     <mergeCell ref="G128:L136"/>
     <mergeCell ref="A137:L137"/>
     <mergeCell ref="A66:L66"/>
@@ -7376,14 +7710,6 @@
     <mergeCell ref="A45:L45"/>
     <mergeCell ref="A36:L36"/>
     <mergeCell ref="A31:L31"/>
-    <mergeCell ref="A24:L24"/>
-    <mergeCell ref="A127:L127"/>
-    <mergeCell ref="A77:L77"/>
-    <mergeCell ref="A97:L97"/>
-    <mergeCell ref="A76:L76"/>
-    <mergeCell ref="A87:L87"/>
-    <mergeCell ref="A107:L107"/>
-    <mergeCell ref="A117:L117"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7414,11 +7740,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
       <c r="D1" s="24"/>
       <c r="E1" s="24"/>
     </row>
@@ -7429,28 +7755,28 @@
       <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:14" ht="15.75">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="46" t="s">
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="47"/>
-      <c r="F3" s="44" t="s">
+      <c r="E3" s="55"/>
+      <c r="F3" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44" t="s">
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="6" t="s">
@@ -7497,22 +7823,22 @@
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="38"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="8">
@@ -7900,11 +8226,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
       <c r="D1" s="26"/>
       <c r="E1" s="26"/>
     </row>
@@ -7915,28 +8241,28 @@
       <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:14" ht="15.75">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="46" t="s">
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="47"/>
-      <c r="F3" s="44" t="s">
+      <c r="E3" s="55"/>
+      <c r="F3" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44" t="s">
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="6" t="s">
@@ -7983,22 +8309,22 @@
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
+      <c r="A5" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="38"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="8">
@@ -8305,11 +8631,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
       <c r="D1" s="25"/>
       <c r="E1" s="25"/>
     </row>
@@ -8320,28 +8646,28 @@
       <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:14" ht="15.75">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="46" t="s">
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="47"/>
-      <c r="F3" s="44" t="s">
+      <c r="E3" s="55"/>
+      <c r="F3" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44" t="s">
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="6" t="s">
@@ -8388,22 +8714,22 @@
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="38"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="8">

</xml_diff>

<commit_message>
Some bug fixes around instantiating Data.Sql classes with Configuration API
</commit_message>
<xml_diff>
--- a/Benchmarks/dotNetRDF BSBM Benchmark.xlsx
+++ b/Benchmarks/dotNetRDF BSBM Benchmark.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="19095" windowHeight="11985"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="19095" windowHeight="11985" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Results (In-Memory)" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="63">
   <si>
     <t>BSBM Benchmarks</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>Leviathan Engine - Version 0.4.2 (With improved internal data structures) using Default Optimiser</t>
+  </si>
+  <si>
+    <t>Leviathan 0.5.0 over dotNetRDF ADO Store using Default Optimiser and Virtualised RDF - Microsoft SQL Server 2008</t>
   </si>
 </sst>
 </file>
@@ -421,7 +424,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -495,6 +498,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -521,9 +539,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -552,23 +567,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -576,6 +579,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1166,11 +1170,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="81735040"/>
-        <c:axId val="81745024"/>
+        <c:axId val="84035840"/>
+        <c:axId val="84041728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="81735040"/>
+        <c:axId val="84035840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1178,14 +1182,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81745024"/>
+        <c:crossAx val="84041728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81745024"/>
+        <c:axId val="84041728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1211,7 +1215,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81735040"/>
+        <c:crossAx val="84035840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1223,7 +1227,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1561,11 +1565,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="81782272"/>
-        <c:axId val="81783808"/>
+        <c:axId val="84218240"/>
+        <c:axId val="84219776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="81782272"/>
+        <c:axId val="84218240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1573,14 +1577,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81783808"/>
+        <c:crossAx val="84219776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81783808"/>
+        <c:axId val="84219776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1606,7 +1610,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81782272"/>
+        <c:crossAx val="84218240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1618,7 +1622,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1824,25 +1828,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="81965056"/>
-        <c:axId val="81966592"/>
+        <c:axId val="84241024"/>
+        <c:axId val="84263296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="81965056"/>
+        <c:axId val="84241024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81966592"/>
+        <c:crossAx val="84263296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81966592"/>
+        <c:axId val="84263296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1867,7 +1871,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81965056"/>
+        <c:crossAx val="84241024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1879,7 +1883,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2211,25 +2215,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="82125184"/>
-        <c:axId val="82126720"/>
+        <c:axId val="84417536"/>
+        <c:axId val="84427520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82125184"/>
+        <c:axId val="84417536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82126720"/>
+        <c:crossAx val="84427520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82126720"/>
+        <c:axId val="84427520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2254,7 +2258,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82125184"/>
+        <c:crossAx val="84417536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2266,7 +2270,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2689,8 +2693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L156"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G154" sqref="G154"/>
     </sheetView>
   </sheetViews>
@@ -2710,34 +2714,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1">
       <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="15.75">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51" t="s">
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51" t="s">
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="6" t="s">
@@ -2778,20 +2782,20 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="50"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="32"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="5">
@@ -2870,20 +2874,20 @@
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="49"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="49"/>
-      <c r="K8" s="49"/>
-      <c r="L8" s="50"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="32"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="8">
@@ -3038,20 +3042,20 @@
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="49"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="49"/>
-      <c r="K13" s="49"/>
-      <c r="L13" s="50"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="32"/>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="5">
@@ -3282,20 +3286,20 @@
       </c>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="48" t="s">
+      <c r="A20" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="49"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="49"/>
-      <c r="J20" s="49"/>
-      <c r="K20" s="49"/>
-      <c r="L20" s="50"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="31"/>
+      <c r="L20" s="32"/>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="8">
@@ -3412,20 +3416,20 @@
       </c>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="48" t="s">
+      <c r="A24" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="49"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="50"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="32"/>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="8">
@@ -3656,20 +3660,20 @@
       </c>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="48" t="s">
+      <c r="A31" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="49"/>
-      <c r="C31" s="49"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="49"/>
-      <c r="F31" s="49"/>
-      <c r="G31" s="49"/>
-      <c r="H31" s="49"/>
-      <c r="I31" s="49"/>
-      <c r="J31" s="49"/>
-      <c r="K31" s="49"/>
-      <c r="L31" s="50"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="31"/>
+      <c r="K31" s="31"/>
+      <c r="L31" s="32"/>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="8">
@@ -3824,20 +3828,20 @@
       </c>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="48" t="s">
+      <c r="A36" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="49"/>
-      <c r="C36" s="49"/>
-      <c r="D36" s="49"/>
-      <c r="E36" s="49"/>
-      <c r="F36" s="49"/>
-      <c r="G36" s="49"/>
-      <c r="H36" s="49"/>
-      <c r="I36" s="49"/>
-      <c r="J36" s="49"/>
-      <c r="K36" s="49"/>
-      <c r="L36" s="50"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="31"/>
+      <c r="I36" s="31"/>
+      <c r="J36" s="31"/>
+      <c r="K36" s="31"/>
+      <c r="L36" s="32"/>
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="8">
@@ -4144,20 +4148,20 @@
       </c>
     </row>
     <row r="45" spans="1:12">
-      <c r="A45" s="38" t="s">
+      <c r="A45" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="B45" s="38"/>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="38"/>
-      <c r="G45" s="38"/>
-      <c r="H45" s="38"/>
-      <c r="I45" s="38"/>
-      <c r="J45" s="38"/>
-      <c r="K45" s="38"/>
-      <c r="L45" s="38"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="29"/>
+      <c r="I45" s="29"/>
+      <c r="J45" s="29"/>
+      <c r="K45" s="29"/>
+      <c r="L45" s="29"/>
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="8">
@@ -4528,20 +4532,20 @@
       <c r="L55" s="8"/>
     </row>
     <row r="56" spans="1:12">
-      <c r="A56" s="52" t="s">
+      <c r="A56" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="B56" s="52"/>
-      <c r="C56" s="52"/>
-      <c r="D56" s="52"/>
-      <c r="E56" s="52"/>
-      <c r="F56" s="52"/>
-      <c r="G56" s="52"/>
-      <c r="H56" s="52"/>
-      <c r="I56" s="52"/>
-      <c r="J56" s="52"/>
-      <c r="K56" s="52"/>
-      <c r="L56" s="52"/>
+      <c r="B56" s="53"/>
+      <c r="C56" s="53"/>
+      <c r="D56" s="53"/>
+      <c r="E56" s="53"/>
+      <c r="F56" s="53"/>
+      <c r="G56" s="53"/>
+      <c r="H56" s="53"/>
+      <c r="I56" s="53"/>
+      <c r="J56" s="53"/>
+      <c r="K56" s="53"/>
+      <c r="L56" s="53"/>
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="19">
@@ -4562,14 +4566,14 @@
       <c r="F57" s="19">
         <v>50</v>
       </c>
-      <c r="G57" s="29" t="s">
+      <c r="G57" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="H57" s="39"/>
-      <c r="I57" s="39"/>
-      <c r="J57" s="39"/>
-      <c r="K57" s="39"/>
-      <c r="L57" s="40"/>
+      <c r="H57" s="43"/>
+      <c r="I57" s="43"/>
+      <c r="J57" s="43"/>
+      <c r="K57" s="43"/>
+      <c r="L57" s="44"/>
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="19">
@@ -4590,12 +4594,12 @@
       <c r="F58" s="19">
         <v>50</v>
       </c>
-      <c r="G58" s="41"/>
-      <c r="H58" s="42"/>
-      <c r="I58" s="42"/>
-      <c r="J58" s="42"/>
-      <c r="K58" s="42"/>
-      <c r="L58" s="43"/>
+      <c r="G58" s="45"/>
+      <c r="H58" s="46"/>
+      <c r="I58" s="46"/>
+      <c r="J58" s="46"/>
+      <c r="K58" s="46"/>
+      <c r="L58" s="47"/>
     </row>
     <row r="59" spans="1:12">
       <c r="A59" s="19">
@@ -4616,12 +4620,12 @@
       <c r="F59" s="19">
         <v>50</v>
       </c>
-      <c r="G59" s="41"/>
-      <c r="H59" s="42"/>
-      <c r="I59" s="42"/>
-      <c r="J59" s="42"/>
-      <c r="K59" s="42"/>
-      <c r="L59" s="43"/>
+      <c r="G59" s="45"/>
+      <c r="H59" s="46"/>
+      <c r="I59" s="46"/>
+      <c r="J59" s="46"/>
+      <c r="K59" s="46"/>
+      <c r="L59" s="47"/>
     </row>
     <row r="60" spans="1:12">
       <c r="A60" s="19">
@@ -4642,12 +4646,12 @@
       <c r="F60" s="19">
         <v>50</v>
       </c>
-      <c r="G60" s="41"/>
-      <c r="H60" s="42"/>
-      <c r="I60" s="42"/>
-      <c r="J60" s="42"/>
-      <c r="K60" s="42"/>
-      <c r="L60" s="43"/>
+      <c r="G60" s="45"/>
+      <c r="H60" s="46"/>
+      <c r="I60" s="46"/>
+      <c r="J60" s="46"/>
+      <c r="K60" s="46"/>
+      <c r="L60" s="47"/>
     </row>
     <row r="61" spans="1:12">
       <c r="A61" s="19">
@@ -4668,12 +4672,12 @@
       <c r="F61" s="19">
         <v>50</v>
       </c>
-      <c r="G61" s="41"/>
-      <c r="H61" s="42"/>
-      <c r="I61" s="42"/>
-      <c r="J61" s="42"/>
-      <c r="K61" s="42"/>
-      <c r="L61" s="43"/>
+      <c r="G61" s="45"/>
+      <c r="H61" s="46"/>
+      <c r="I61" s="46"/>
+      <c r="J61" s="46"/>
+      <c r="K61" s="46"/>
+      <c r="L61" s="47"/>
     </row>
     <row r="62" spans="1:12">
       <c r="A62" s="19">
@@ -4694,12 +4698,12 @@
       <c r="F62" s="19">
         <v>50</v>
       </c>
-      <c r="G62" s="41"/>
-      <c r="H62" s="42"/>
-      <c r="I62" s="42"/>
-      <c r="J62" s="42"/>
-      <c r="K62" s="42"/>
-      <c r="L62" s="43"/>
+      <c r="G62" s="45"/>
+      <c r="H62" s="46"/>
+      <c r="I62" s="46"/>
+      <c r="J62" s="46"/>
+      <c r="K62" s="46"/>
+      <c r="L62" s="47"/>
     </row>
     <row r="63" spans="1:12">
       <c r="A63" s="22">
@@ -4720,12 +4724,12 @@
       <c r="F63" s="19">
         <v>50</v>
       </c>
-      <c r="G63" s="41"/>
-      <c r="H63" s="42"/>
-      <c r="I63" s="42"/>
-      <c r="J63" s="42"/>
-      <c r="K63" s="42"/>
-      <c r="L63" s="43"/>
+      <c r="G63" s="45"/>
+      <c r="H63" s="46"/>
+      <c r="I63" s="46"/>
+      <c r="J63" s="46"/>
+      <c r="K63" s="46"/>
+      <c r="L63" s="47"/>
     </row>
     <row r="64" spans="1:12">
       <c r="A64" s="22">
@@ -4746,12 +4750,12 @@
       <c r="F64" s="19">
         <v>50</v>
       </c>
-      <c r="G64" s="44"/>
-      <c r="H64" s="45"/>
-      <c r="I64" s="45"/>
-      <c r="J64" s="45"/>
-      <c r="K64" s="45"/>
-      <c r="L64" s="46"/>
+      <c r="G64" s="48"/>
+      <c r="H64" s="49"/>
+      <c r="I64" s="49"/>
+      <c r="J64" s="49"/>
+      <c r="K64" s="49"/>
+      <c r="L64" s="50"/>
     </row>
     <row r="65" spans="1:12">
       <c r="A65" s="22">
@@ -4792,20 +4796,20 @@
       </c>
     </row>
     <row r="66" spans="1:12">
-      <c r="A66" s="38" t="s">
+      <c r="A66" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="B66" s="38"/>
-      <c r="C66" s="38"/>
-      <c r="D66" s="38"/>
-      <c r="E66" s="38"/>
-      <c r="F66" s="38"/>
-      <c r="G66" s="38"/>
-      <c r="H66" s="38"/>
-      <c r="I66" s="38"/>
-      <c r="J66" s="38"/>
-      <c r="K66" s="38"/>
-      <c r="L66" s="38"/>
+      <c r="B66" s="29"/>
+      <c r="C66" s="29"/>
+      <c r="D66" s="29"/>
+      <c r="E66" s="29"/>
+      <c r="F66" s="29"/>
+      <c r="G66" s="29"/>
+      <c r="H66" s="29"/>
+      <c r="I66" s="29"/>
+      <c r="J66" s="29"/>
+      <c r="K66" s="29"/>
+      <c r="L66" s="29"/>
     </row>
     <row r="67" spans="1:12">
       <c r="A67" s="8">
@@ -5150,36 +5154,36 @@
       </c>
     </row>
     <row r="76" spans="1:12" ht="30" customHeight="1">
-      <c r="A76" s="53" t="s">
+      <c r="A76" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B76" s="53"/>
-      <c r="C76" s="53"/>
-      <c r="D76" s="53"/>
-      <c r="E76" s="53"/>
-      <c r="F76" s="53"/>
-      <c r="G76" s="53"/>
-      <c r="H76" s="53"/>
-      <c r="I76" s="53"/>
-      <c r="J76" s="53"/>
-      <c r="K76" s="53"/>
-      <c r="L76" s="53"/>
+      <c r="B76" s="33"/>
+      <c r="C76" s="33"/>
+      <c r="D76" s="33"/>
+      <c r="E76" s="33"/>
+      <c r="F76" s="33"/>
+      <c r="G76" s="33"/>
+      <c r="H76" s="33"/>
+      <c r="I76" s="33"/>
+      <c r="J76" s="33"/>
+      <c r="K76" s="33"/>
+      <c r="L76" s="33"/>
     </row>
     <row r="77" spans="1:12">
-      <c r="A77" s="38" t="s">
+      <c r="A77" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="B77" s="38"/>
-      <c r="C77" s="38"/>
-      <c r="D77" s="38"/>
-      <c r="E77" s="38"/>
-      <c r="F77" s="38"/>
-      <c r="G77" s="38"/>
-      <c r="H77" s="38"/>
-      <c r="I77" s="38"/>
-      <c r="J77" s="38"/>
-      <c r="K77" s="38"/>
-      <c r="L77" s="38"/>
+      <c r="B77" s="29"/>
+      <c r="C77" s="29"/>
+      <c r="D77" s="29"/>
+      <c r="E77" s="29"/>
+      <c r="F77" s="29"/>
+      <c r="G77" s="29"/>
+      <c r="H77" s="29"/>
+      <c r="I77" s="29"/>
+      <c r="J77" s="29"/>
+      <c r="K77" s="29"/>
+      <c r="L77" s="29"/>
     </row>
     <row r="78" spans="1:12">
       <c r="A78" s="8">
@@ -5500,20 +5504,20 @@
       <c r="L86" s="8"/>
     </row>
     <row r="87" spans="1:12">
-      <c r="A87" s="38" t="s">
+      <c r="A87" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="B87" s="38"/>
-      <c r="C87" s="38"/>
-      <c r="D87" s="38"/>
-      <c r="E87" s="38"/>
-      <c r="F87" s="38"/>
-      <c r="G87" s="38"/>
-      <c r="H87" s="38"/>
-      <c r="I87" s="38"/>
-      <c r="J87" s="38"/>
-      <c r="K87" s="38"/>
-      <c r="L87" s="38"/>
+      <c r="B87" s="29"/>
+      <c r="C87" s="29"/>
+      <c r="D87" s="29"/>
+      <c r="E87" s="29"/>
+      <c r="F87" s="29"/>
+      <c r="G87" s="29"/>
+      <c r="H87" s="29"/>
+      <c r="I87" s="29"/>
+      <c r="J87" s="29"/>
+      <c r="K87" s="29"/>
+      <c r="L87" s="29"/>
     </row>
     <row r="88" spans="1:12">
       <c r="A88" s="8">
@@ -5810,20 +5814,20 @@
       <c r="L96" s="8"/>
     </row>
     <row r="97" spans="1:12">
-      <c r="A97" s="38" t="s">
+      <c r="A97" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="B97" s="38"/>
-      <c r="C97" s="38"/>
-      <c r="D97" s="38"/>
-      <c r="E97" s="38"/>
-      <c r="F97" s="38"/>
-      <c r="G97" s="38"/>
-      <c r="H97" s="38"/>
-      <c r="I97" s="38"/>
-      <c r="J97" s="38"/>
-      <c r="K97" s="38"/>
-      <c r="L97" s="38"/>
+      <c r="B97" s="29"/>
+      <c r="C97" s="29"/>
+      <c r="D97" s="29"/>
+      <c r="E97" s="29"/>
+      <c r="F97" s="29"/>
+      <c r="G97" s="29"/>
+      <c r="H97" s="29"/>
+      <c r="I97" s="29"/>
+      <c r="J97" s="29"/>
+      <c r="K97" s="29"/>
+      <c r="L97" s="29"/>
     </row>
     <row r="98" spans="1:12">
       <c r="A98" s="8">
@@ -6144,20 +6148,20 @@
       <c r="L106" s="8"/>
     </row>
     <row r="107" spans="1:12">
-      <c r="A107" s="38" t="s">
+      <c r="A107" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="B107" s="38"/>
-      <c r="C107" s="38"/>
-      <c r="D107" s="38"/>
-      <c r="E107" s="38"/>
-      <c r="F107" s="38"/>
-      <c r="G107" s="38"/>
-      <c r="H107" s="38"/>
-      <c r="I107" s="38"/>
-      <c r="J107" s="38"/>
-      <c r="K107" s="38"/>
-      <c r="L107" s="38"/>
+      <c r="B107" s="29"/>
+      <c r="C107" s="29"/>
+      <c r="D107" s="29"/>
+      <c r="E107" s="29"/>
+      <c r="F107" s="29"/>
+      <c r="G107" s="29"/>
+      <c r="H107" s="29"/>
+      <c r="I107" s="29"/>
+      <c r="J107" s="29"/>
+      <c r="K107" s="29"/>
+      <c r="L107" s="29"/>
     </row>
     <row r="108" spans="1:12">
       <c r="A108" s="8">
@@ -6454,20 +6458,20 @@
       <c r="L116" s="8"/>
     </row>
     <row r="117" spans="1:12">
-      <c r="A117" s="38" t="s">
+      <c r="A117" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="B117" s="38"/>
-      <c r="C117" s="38"/>
-      <c r="D117" s="38"/>
-      <c r="E117" s="38"/>
-      <c r="F117" s="38"/>
-      <c r="G117" s="38"/>
-      <c r="H117" s="38"/>
-      <c r="I117" s="38"/>
-      <c r="J117" s="38"/>
-      <c r="K117" s="38"/>
-      <c r="L117" s="38"/>
+      <c r="B117" s="29"/>
+      <c r="C117" s="29"/>
+      <c r="D117" s="29"/>
+      <c r="E117" s="29"/>
+      <c r="F117" s="29"/>
+      <c r="G117" s="29"/>
+      <c r="H117" s="29"/>
+      <c r="I117" s="29"/>
+      <c r="J117" s="29"/>
+      <c r="K117" s="29"/>
+      <c r="L117" s="29"/>
     </row>
     <row r="118" spans="1:12">
       <c r="A118" s="8">
@@ -6788,20 +6792,20 @@
       <c r="L126" s="3"/>
     </row>
     <row r="127" spans="1:12">
-      <c r="A127" s="38" t="s">
+      <c r="A127" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="B127" s="38"/>
-      <c r="C127" s="38"/>
-      <c r="D127" s="38"/>
-      <c r="E127" s="38"/>
-      <c r="F127" s="38"/>
-      <c r="G127" s="38"/>
-      <c r="H127" s="38"/>
-      <c r="I127" s="38"/>
-      <c r="J127" s="38"/>
-      <c r="K127" s="38"/>
-      <c r="L127" s="38"/>
+      <c r="B127" s="29"/>
+      <c r="C127" s="29"/>
+      <c r="D127" s="29"/>
+      <c r="E127" s="29"/>
+      <c r="F127" s="29"/>
+      <c r="G127" s="29"/>
+      <c r="H127" s="29"/>
+      <c r="I127" s="29"/>
+      <c r="J127" s="29"/>
+      <c r="K127" s="29"/>
+      <c r="L127" s="29"/>
     </row>
     <row r="128" spans="1:12">
       <c r="A128" s="19">
@@ -6822,14 +6826,14 @@
       <c r="F128" s="19">
         <v>50</v>
       </c>
-      <c r="G128" s="29" t="s">
+      <c r="G128" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="H128" s="30"/>
-      <c r="I128" s="30"/>
-      <c r="J128" s="30"/>
-      <c r="K128" s="30"/>
-      <c r="L128" s="31"/>
+      <c r="H128" s="35"/>
+      <c r="I128" s="35"/>
+      <c r="J128" s="35"/>
+      <c r="K128" s="35"/>
+      <c r="L128" s="36"/>
     </row>
     <row r="129" spans="1:12">
       <c r="A129" s="19">
@@ -6850,12 +6854,12 @@
       <c r="F129" s="19">
         <v>50</v>
       </c>
-      <c r="G129" s="32"/>
-      <c r="H129" s="33"/>
-      <c r="I129" s="33"/>
-      <c r="J129" s="33"/>
-      <c r="K129" s="33"/>
-      <c r="L129" s="34"/>
+      <c r="G129" s="37"/>
+      <c r="H129" s="38"/>
+      <c r="I129" s="38"/>
+      <c r="J129" s="38"/>
+      <c r="K129" s="38"/>
+      <c r="L129" s="39"/>
     </row>
     <row r="130" spans="1:12">
       <c r="A130" s="19">
@@ -6876,12 +6880,12 @@
       <c r="F130" s="19">
         <v>50</v>
       </c>
-      <c r="G130" s="32"/>
-      <c r="H130" s="33"/>
-      <c r="I130" s="33"/>
-      <c r="J130" s="33"/>
-      <c r="K130" s="33"/>
-      <c r="L130" s="34"/>
+      <c r="G130" s="37"/>
+      <c r="H130" s="38"/>
+      <c r="I130" s="38"/>
+      <c r="J130" s="38"/>
+      <c r="K130" s="38"/>
+      <c r="L130" s="39"/>
     </row>
     <row r="131" spans="1:12">
       <c r="A131" s="19">
@@ -6902,12 +6906,12 @@
       <c r="F131" s="19">
         <v>50</v>
       </c>
-      <c r="G131" s="32"/>
-      <c r="H131" s="33"/>
-      <c r="I131" s="33"/>
-      <c r="J131" s="33"/>
-      <c r="K131" s="33"/>
-      <c r="L131" s="34"/>
+      <c r="G131" s="37"/>
+      <c r="H131" s="38"/>
+      <c r="I131" s="38"/>
+      <c r="J131" s="38"/>
+      <c r="K131" s="38"/>
+      <c r="L131" s="39"/>
     </row>
     <row r="132" spans="1:12">
       <c r="A132" s="19">
@@ -6928,12 +6932,12 @@
       <c r="F132" s="19">
         <v>50</v>
       </c>
-      <c r="G132" s="32"/>
-      <c r="H132" s="33"/>
-      <c r="I132" s="33"/>
-      <c r="J132" s="33"/>
-      <c r="K132" s="33"/>
-      <c r="L132" s="34"/>
+      <c r="G132" s="37"/>
+      <c r="H132" s="38"/>
+      <c r="I132" s="38"/>
+      <c r="J132" s="38"/>
+      <c r="K132" s="38"/>
+      <c r="L132" s="39"/>
     </row>
     <row r="133" spans="1:12">
       <c r="A133" s="19">
@@ -6954,12 +6958,12 @@
       <c r="F133" s="19">
         <v>50</v>
       </c>
-      <c r="G133" s="32"/>
-      <c r="H133" s="33"/>
-      <c r="I133" s="33"/>
-      <c r="J133" s="33"/>
-      <c r="K133" s="33"/>
-      <c r="L133" s="34"/>
+      <c r="G133" s="37"/>
+      <c r="H133" s="38"/>
+      <c r="I133" s="38"/>
+      <c r="J133" s="38"/>
+      <c r="K133" s="38"/>
+      <c r="L133" s="39"/>
     </row>
     <row r="134" spans="1:12">
       <c r="A134" s="22">
@@ -6980,12 +6984,12 @@
       <c r="F134" s="19">
         <v>50</v>
       </c>
-      <c r="G134" s="32"/>
-      <c r="H134" s="33"/>
-      <c r="I134" s="33"/>
-      <c r="J134" s="33"/>
-      <c r="K134" s="33"/>
-      <c r="L134" s="34"/>
+      <c r="G134" s="37"/>
+      <c r="H134" s="38"/>
+      <c r="I134" s="38"/>
+      <c r="J134" s="38"/>
+      <c r="K134" s="38"/>
+      <c r="L134" s="39"/>
     </row>
     <row r="135" spans="1:12">
       <c r="A135" s="22">
@@ -7006,12 +7010,12 @@
       <c r="F135" s="19">
         <v>50</v>
       </c>
-      <c r="G135" s="32"/>
-      <c r="H135" s="33"/>
-      <c r="I135" s="33"/>
-      <c r="J135" s="33"/>
-      <c r="K135" s="33"/>
-      <c r="L135" s="34"/>
+      <c r="G135" s="37"/>
+      <c r="H135" s="38"/>
+      <c r="I135" s="38"/>
+      <c r="J135" s="38"/>
+      <c r="K135" s="38"/>
+      <c r="L135" s="39"/>
     </row>
     <row r="136" spans="1:12">
       <c r="A136" s="22">
@@ -7032,28 +7036,28 @@
       <c r="F136" s="19">
         <v>50</v>
       </c>
-      <c r="G136" s="35"/>
-      <c r="H136" s="36"/>
-      <c r="I136" s="36"/>
-      <c r="J136" s="36"/>
-      <c r="K136" s="36"/>
-      <c r="L136" s="37"/>
+      <c r="G136" s="40"/>
+      <c r="H136" s="41"/>
+      <c r="I136" s="41"/>
+      <c r="J136" s="41"/>
+      <c r="K136" s="41"/>
+      <c r="L136" s="42"/>
     </row>
     <row r="137" spans="1:12">
-      <c r="A137" s="38" t="s">
+      <c r="A137" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="B137" s="38"/>
-      <c r="C137" s="38"/>
-      <c r="D137" s="38"/>
-      <c r="E137" s="38"/>
-      <c r="F137" s="38"/>
-      <c r="G137" s="38"/>
-      <c r="H137" s="38"/>
-      <c r="I137" s="38"/>
-      <c r="J137" s="38"/>
-      <c r="K137" s="38"/>
-      <c r="L137" s="38"/>
+      <c r="B137" s="29"/>
+      <c r="C137" s="29"/>
+      <c r="D137" s="29"/>
+      <c r="E137" s="29"/>
+      <c r="F137" s="29"/>
+      <c r="G137" s="29"/>
+      <c r="H137" s="29"/>
+      <c r="I137" s="29"/>
+      <c r="J137" s="29"/>
+      <c r="K137" s="29"/>
+      <c r="L137" s="29"/>
     </row>
     <row r="138" spans="1:12">
       <c r="A138" s="8">
@@ -7362,20 +7366,20 @@
       <c r="L146" s="3"/>
     </row>
     <row r="147" spans="1:12">
-      <c r="A147" s="38" t="s">
+      <c r="A147" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B147" s="38"/>
-      <c r="C147" s="38"/>
-      <c r="D147" s="38"/>
-      <c r="E147" s="38"/>
-      <c r="F147" s="38"/>
-      <c r="G147" s="38"/>
-      <c r="H147" s="38"/>
-      <c r="I147" s="38"/>
-      <c r="J147" s="38"/>
-      <c r="K147" s="38"/>
-      <c r="L147" s="38"/>
+      <c r="B147" s="29"/>
+      <c r="C147" s="29"/>
+      <c r="D147" s="29"/>
+      <c r="E147" s="29"/>
+      <c r="F147" s="29"/>
+      <c r="G147" s="29"/>
+      <c r="H147" s="29"/>
+      <c r="I147" s="29"/>
+      <c r="J147" s="29"/>
+      <c r="K147" s="29"/>
+      <c r="L147" s="29"/>
     </row>
     <row r="148" spans="1:12">
       <c r="A148" s="8">
@@ -7685,6 +7689,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A31:L31"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="A20:L20"/>
+    <mergeCell ref="A13:L13"/>
+    <mergeCell ref="A8:L8"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="G3:L3"/>
     <mergeCell ref="A147:L147"/>
     <mergeCell ref="A24:L24"/>
     <mergeCell ref="A127:L127"/>
@@ -7698,18 +7711,9 @@
     <mergeCell ref="A137:L137"/>
     <mergeCell ref="A66:L66"/>
     <mergeCell ref="G57:L64"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A5:L5"/>
-    <mergeCell ref="A20:L20"/>
-    <mergeCell ref="A13:L13"/>
-    <mergeCell ref="A8:L8"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="G3:L3"/>
     <mergeCell ref="A56:L56"/>
     <mergeCell ref="A45:L45"/>
     <mergeCell ref="A36:L36"/>
-    <mergeCell ref="A31:L31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7740,11 +7744,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
       <c r="D1" s="24"/>
       <c r="E1" s="24"/>
     </row>
@@ -7755,28 +7759,28 @@
       <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:14" ht="15.75">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
       <c r="D3" s="54" t="s">
         <v>44</v>
       </c>
       <c r="E3" s="55"/>
-      <c r="F3" s="51" t="s">
+      <c r="F3" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51" t="s">
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="6" t="s">
@@ -7823,22 +7827,22 @@
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="8">
@@ -8226,11 +8230,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
       <c r="D1" s="26"/>
       <c r="E1" s="26"/>
     </row>
@@ -8241,28 +8245,28 @@
       <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:14" ht="15.75">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
       <c r="D3" s="54" t="s">
         <v>44</v>
       </c>
       <c r="E3" s="55"/>
-      <c r="F3" s="51" t="s">
+      <c r="F3" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51" t="s">
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="6" t="s">
@@ -8309,22 +8313,22 @@
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38"/>
+      <c r="A5" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="8">
@@ -8609,17 +8613,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6:K9"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
@@ -8627,15 +8631,16 @@
     <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
       <c r="D1" s="25"/>
       <c r="E1" s="25"/>
     </row>
@@ -8646,28 +8651,28 @@
       <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:14" ht="15.75">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
       <c r="D3" s="54" t="s">
         <v>44</v>
       </c>
       <c r="E3" s="55"/>
-      <c r="F3" s="51" t="s">
+      <c r="F3" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51" t="s">
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="6" t="s">
@@ -8714,22 +8719,22 @@
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="8">
@@ -9047,8 +9052,339 @@
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
     </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="29"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="8">
+        <v>10</v>
+      </c>
+      <c r="B16" s="9">
+        <v>4991</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="8">
+        <v>2500</v>
+      </c>
+      <c r="G16" s="8">
+        <v>10</v>
+      </c>
+      <c r="H16" s="8">
+        <v>50</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0.1026</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0.18459999999999999</v>
+      </c>
+      <c r="K16" s="3">
+        <v>5.6280000000000001</v>
+      </c>
+      <c r="L16" s="3">
+        <v>31983.3</v>
+      </c>
+      <c r="M16" s="3">
+        <v>0.11255999999999999</v>
+      </c>
+      <c r="N16" s="3">
+        <v>0.11179</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="8">
+        <v>50</v>
+      </c>
+      <c r="B17" s="9">
+        <v>22716</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="8">
+        <v>2500</v>
+      </c>
+      <c r="G17" s="8">
+        <v>10</v>
+      </c>
+      <c r="H17" s="8">
+        <v>50</v>
+      </c>
+      <c r="I17" s="3">
+        <v>0.13739999999999999</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0.25929999999999997</v>
+      </c>
+      <c r="K17" s="3">
+        <v>8.1020000000000003</v>
+      </c>
+      <c r="L17" s="56">
+        <v>22215.73</v>
+      </c>
+      <c r="M17" s="3">
+        <v>0.16205</v>
+      </c>
+      <c r="N17" s="3">
+        <v>0.15948000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="8">
+        <v>100</v>
+      </c>
+      <c r="B18" s="9">
+        <v>40333</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="8">
+        <v>2500</v>
+      </c>
+      <c r="G18" s="8">
+        <v>10</v>
+      </c>
+      <c r="H18" s="8">
+        <v>50</v>
+      </c>
+      <c r="I18" s="3">
+        <v>0.1908</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0.43340000000000001</v>
+      </c>
+      <c r="K18" s="3">
+        <v>12.023</v>
+      </c>
+      <c r="L18" s="3">
+        <v>14971.51</v>
+      </c>
+      <c r="M18" s="3">
+        <v>0.24046000000000001</v>
+      </c>
+      <c r="N18" s="3">
+        <v>0.23547999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="8">
+        <v>250</v>
+      </c>
+      <c r="B19" s="9">
+        <v>98113</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="8">
+        <v>2500</v>
+      </c>
+      <c r="G19" s="8">
+        <v>10</v>
+      </c>
+      <c r="H19" s="8">
+        <v>50</v>
+      </c>
+      <c r="I19" s="3">
+        <v>0.41320000000000001</v>
+      </c>
+      <c r="J19" s="3">
+        <v>1.1180000000000001</v>
+      </c>
+      <c r="K19" s="3">
+        <v>28.995000000000001</v>
+      </c>
+      <c r="L19" s="3">
+        <v>6208.04</v>
+      </c>
+      <c r="M19" s="3">
+        <v>0.57989000000000002</v>
+      </c>
+      <c r="N19" s="3">
+        <v>0.56594</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="8">
+        <v>500</v>
+      </c>
+      <c r="B20" s="9">
+        <v>191502</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="8">
+        <v>2500</v>
+      </c>
+      <c r="G20" s="8">
+        <v>10</v>
+      </c>
+      <c r="H20" s="8">
+        <v>50</v>
+      </c>
+      <c r="I20" s="3">
+        <v>1.0196000000000001</v>
+      </c>
+      <c r="J20" s="3">
+        <v>4.8540999999999999</v>
+      </c>
+      <c r="K20" s="3">
+        <v>78.183000000000007</v>
+      </c>
+      <c r="L20" s="3">
+        <v>2302.2800000000002</v>
+      </c>
+      <c r="M20" s="3">
+        <v>1.5636699999999999</v>
+      </c>
+      <c r="N20" s="3">
+        <v>1.5053399999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="8">
+        <v>1000</v>
+      </c>
+      <c r="B21" s="9">
+        <v>375114</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="8">
+        <v>2500</v>
+      </c>
+      <c r="G21" s="8">
+        <v>10</v>
+      </c>
+      <c r="H21" s="8">
+        <v>50</v>
+      </c>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="5">
+        <v>1500</v>
+      </c>
+      <c r="B22" s="7">
+        <v>550078</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="5">
+        <v>2500</v>
+      </c>
+      <c r="G22" s="8">
+        <v>10</v>
+      </c>
+      <c r="H22" s="8">
+        <v>50</v>
+      </c>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="5">
+        <v>2000</v>
+      </c>
+      <c r="B23" s="7">
+        <v>725515</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="5">
+        <v>2500</v>
+      </c>
+      <c r="G23" s="8">
+        <v>10</v>
+      </c>
+      <c r="H23" s="8">
+        <v>50</v>
+      </c>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="5">
+        <v>2500</v>
+      </c>
+      <c r="B24" s="7">
+        <v>900517</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="5">
+        <v>2500</v>
+      </c>
+      <c r="G24" s="8">
+        <v>10</v>
+      </c>
+      <c r="H24" s="8">
+        <v>50</v>
+      </c>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A15:N15"/>
     <mergeCell ref="A5:N5"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A3:C3"/>
@@ -9057,6 +9393,7 @@
     <mergeCell ref="I3:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Some experimentation re: CORE-73 Has some effect on speed but needs to be used more sparingly to get the best effect I think, needs further experimentation and left disabled currently Affects Issue [73]
</commit_message>
<xml_diff>
--- a/Benchmarks/dotNetRDF BSBM Benchmark.xlsx
+++ b/Benchmarks/dotNetRDF BSBM Benchmark.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="19095" windowHeight="11985" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="19095" windowHeight="11985"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Results (In-Memory)" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="64">
   <si>
     <t>BSBM Benchmarks</t>
   </si>
@@ -192,22 +192,25 @@
     <t>Leviathan Engine - Version 0.4.1 using Statistics Optimiser with 4 Clients</t>
   </si>
   <si>
-    <t>Leviathan Engine - Version 0.4.2 (Non-rigorous evaluation) using Default Optimiser</t>
-  </si>
-  <si>
     <t>Results here are considered suspect as analysis suggested they were incorrect.  Non-rigorous evaluation strategy has been removed from the engine</t>
   </si>
   <si>
-    <t>Leviathan Engine - Version 0.4.2 (Basic Optimisations) using Default Optimiser</t>
+    <t>Leviathan 0.5.0 over dotNetRDF ADO Store using Default Optimiser and Virtualised RDF - Microsoft SQL Server 2008</t>
   </si>
   <si>
-    <t>Leviathan Engine - Version 0.4.2 (With Identity Filter optimisation enabled) using Default Optimiser</t>
+    <t>Leviathan Engine - Version 0.5.0 (Basic Optimisations) using Default Optimiser</t>
   </si>
   <si>
-    <t>Leviathan Engine - Version 0.4.2 (With improved internal data structures) using Default Optimiser</t>
+    <t>Leviathan Engine - Version 0.5.0 (Non-rigorous evaluation) using Default Optimiser</t>
   </si>
   <si>
-    <t>Leviathan 0.5.0 over dotNetRDF ADO Store using Default Optimiser and Virtualised RDF - Microsoft SQL Server 2008</t>
+    <t>Leviathan Engine - Version 0.5.0 (With Identity Filter optimisation enabled) using Default Optimiser</t>
+  </si>
+  <si>
+    <t>Leviathan Engine - Version 0.5.0 (With improved internal data structures) using Default Optimiser</t>
+  </si>
+  <si>
+    <t>Leviathan Engine - Version 0.5.1 (With experimental join speed boost optimisation) using Default Optimiser</t>
   </si>
 </sst>
 </file>
@@ -498,9 +501,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -508,6 +509,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -564,12 +574,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -579,7 +583,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1170,11 +1173,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="84035840"/>
-        <c:axId val="84041728"/>
+        <c:axId val="77498624"/>
+        <c:axId val="77504512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84035840"/>
+        <c:axId val="77498624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1182,14 +1185,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84041728"/>
+        <c:crossAx val="77504512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84041728"/>
+        <c:axId val="77504512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1215,7 +1218,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84035840"/>
+        <c:crossAx val="77498624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1227,7 +1230,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1565,11 +1568,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="84218240"/>
-        <c:axId val="84219776"/>
+        <c:axId val="77029760"/>
+        <c:axId val="77031296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84218240"/>
+        <c:axId val="77029760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1577,14 +1580,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84219776"/>
+        <c:crossAx val="77031296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84219776"/>
+        <c:axId val="77031296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1610,7 +1613,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84218240"/>
+        <c:crossAx val="77029760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1622,7 +1625,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1828,25 +1831,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="84241024"/>
-        <c:axId val="84263296"/>
+        <c:axId val="77732480"/>
+        <c:axId val="77734272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84241024"/>
+        <c:axId val="77732480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84263296"/>
+        <c:crossAx val="77734272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84263296"/>
+        <c:axId val="77734272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1871,7 +1874,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84241024"/>
+        <c:crossAx val="77732480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1883,7 +1886,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2215,25 +2218,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="84417536"/>
-        <c:axId val="84427520"/>
+        <c:axId val="78068736"/>
+        <c:axId val="78095104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84417536"/>
+        <c:axId val="78068736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84427520"/>
+        <c:crossAx val="78095104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84427520"/>
+        <c:axId val="78095104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2258,7 +2261,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84417536"/>
+        <c:crossAx val="78068736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2270,7 +2273,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2691,11 +2694,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L156"/>
+  <dimension ref="A1:L166"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G154" sqref="G154"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G163" sqref="G163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2714,34 +2717,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1">
       <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="15.75">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52" t="s">
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="6" t="s">
@@ -4148,20 +4151,20 @@
       </c>
     </row>
     <row r="45" spans="1:12">
-      <c r="A45" s="29" t="s">
+      <c r="A45" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="29"/>
-      <c r="G45" s="29"/>
-      <c r="H45" s="29"/>
-      <c r="I45" s="29"/>
-      <c r="J45" s="29"/>
-      <c r="K45" s="29"/>
-      <c r="L45" s="29"/>
+      <c r="B45" s="35"/>
+      <c r="C45" s="35"/>
+      <c r="D45" s="35"/>
+      <c r="E45" s="35"/>
+      <c r="F45" s="35"/>
+      <c r="G45" s="35"/>
+      <c r="H45" s="35"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="35"/>
+      <c r="K45" s="35"/>
+      <c r="L45" s="35"/>
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="8">
@@ -4532,20 +4535,20 @@
       <c r="L55" s="8"/>
     </row>
     <row r="56" spans="1:12">
-      <c r="A56" s="53" t="s">
+      <c r="A56" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="B56" s="53"/>
-      <c r="C56" s="53"/>
-      <c r="D56" s="53"/>
-      <c r="E56" s="53"/>
-      <c r="F56" s="53"/>
-      <c r="G56" s="53"/>
-      <c r="H56" s="53"/>
-      <c r="I56" s="53"/>
-      <c r="J56" s="53"/>
-      <c r="K56" s="53"/>
-      <c r="L56" s="53"/>
+      <c r="B56" s="54"/>
+      <c r="C56" s="54"/>
+      <c r="D56" s="54"/>
+      <c r="E56" s="54"/>
+      <c r="F56" s="54"/>
+      <c r="G56" s="54"/>
+      <c r="H56" s="54"/>
+      <c r="I56" s="54"/>
+      <c r="J56" s="54"/>
+      <c r="K56" s="54"/>
+      <c r="L56" s="54"/>
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="19">
@@ -4566,14 +4569,14 @@
       <c r="F57" s="19">
         <v>50</v>
       </c>
-      <c r="G57" s="34" t="s">
+      <c r="G57" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="H57" s="43"/>
-      <c r="I57" s="43"/>
-      <c r="J57" s="43"/>
-      <c r="K57" s="43"/>
-      <c r="L57" s="44"/>
+      <c r="H57" s="46"/>
+      <c r="I57" s="46"/>
+      <c r="J57" s="46"/>
+      <c r="K57" s="46"/>
+      <c r="L57" s="47"/>
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="19">
@@ -4594,12 +4597,12 @@
       <c r="F58" s="19">
         <v>50</v>
       </c>
-      <c r="G58" s="45"/>
-      <c r="H58" s="46"/>
-      <c r="I58" s="46"/>
-      <c r="J58" s="46"/>
-      <c r="K58" s="46"/>
-      <c r="L58" s="47"/>
+      <c r="G58" s="48"/>
+      <c r="H58" s="49"/>
+      <c r="I58" s="49"/>
+      <c r="J58" s="49"/>
+      <c r="K58" s="49"/>
+      <c r="L58" s="50"/>
     </row>
     <row r="59" spans="1:12">
       <c r="A59" s="19">
@@ -4620,12 +4623,12 @@
       <c r="F59" s="19">
         <v>50</v>
       </c>
-      <c r="G59" s="45"/>
-      <c r="H59" s="46"/>
-      <c r="I59" s="46"/>
-      <c r="J59" s="46"/>
-      <c r="K59" s="46"/>
-      <c r="L59" s="47"/>
+      <c r="G59" s="48"/>
+      <c r="H59" s="49"/>
+      <c r="I59" s="49"/>
+      <c r="J59" s="49"/>
+      <c r="K59" s="49"/>
+      <c r="L59" s="50"/>
     </row>
     <row r="60" spans="1:12">
       <c r="A60" s="19">
@@ -4646,12 +4649,12 @@
       <c r="F60" s="19">
         <v>50</v>
       </c>
-      <c r="G60" s="45"/>
-      <c r="H60" s="46"/>
-      <c r="I60" s="46"/>
-      <c r="J60" s="46"/>
-      <c r="K60" s="46"/>
-      <c r="L60" s="47"/>
+      <c r="G60" s="48"/>
+      <c r="H60" s="49"/>
+      <c r="I60" s="49"/>
+      <c r="J60" s="49"/>
+      <c r="K60" s="49"/>
+      <c r="L60" s="50"/>
     </row>
     <row r="61" spans="1:12">
       <c r="A61" s="19">
@@ -4672,12 +4675,12 @@
       <c r="F61" s="19">
         <v>50</v>
       </c>
-      <c r="G61" s="45"/>
-      <c r="H61" s="46"/>
-      <c r="I61" s="46"/>
-      <c r="J61" s="46"/>
-      <c r="K61" s="46"/>
-      <c r="L61" s="47"/>
+      <c r="G61" s="48"/>
+      <c r="H61" s="49"/>
+      <c r="I61" s="49"/>
+      <c r="J61" s="49"/>
+      <c r="K61" s="49"/>
+      <c r="L61" s="50"/>
     </row>
     <row r="62" spans="1:12">
       <c r="A62" s="19">
@@ -4698,12 +4701,12 @@
       <c r="F62" s="19">
         <v>50</v>
       </c>
-      <c r="G62" s="45"/>
-      <c r="H62" s="46"/>
-      <c r="I62" s="46"/>
-      <c r="J62" s="46"/>
-      <c r="K62" s="46"/>
-      <c r="L62" s="47"/>
+      <c r="G62" s="48"/>
+      <c r="H62" s="49"/>
+      <c r="I62" s="49"/>
+      <c r="J62" s="49"/>
+      <c r="K62" s="49"/>
+      <c r="L62" s="50"/>
     </row>
     <row r="63" spans="1:12">
       <c r="A63" s="22">
@@ -4724,12 +4727,12 @@
       <c r="F63" s="19">
         <v>50</v>
       </c>
-      <c r="G63" s="45"/>
-      <c r="H63" s="46"/>
-      <c r="I63" s="46"/>
-      <c r="J63" s="46"/>
-      <c r="K63" s="46"/>
-      <c r="L63" s="47"/>
+      <c r="G63" s="48"/>
+      <c r="H63" s="49"/>
+      <c r="I63" s="49"/>
+      <c r="J63" s="49"/>
+      <c r="K63" s="49"/>
+      <c r="L63" s="50"/>
     </row>
     <row r="64" spans="1:12">
       <c r="A64" s="22">
@@ -4750,12 +4753,12 @@
       <c r="F64" s="19">
         <v>50</v>
       </c>
-      <c r="G64" s="48"/>
-      <c r="H64" s="49"/>
-      <c r="I64" s="49"/>
-      <c r="J64" s="49"/>
-      <c r="K64" s="49"/>
-      <c r="L64" s="50"/>
+      <c r="G64" s="51"/>
+      <c r="H64" s="52"/>
+      <c r="I64" s="52"/>
+      <c r="J64" s="52"/>
+      <c r="K64" s="52"/>
+      <c r="L64" s="53"/>
     </row>
     <row r="65" spans="1:12">
       <c r="A65" s="22">
@@ -4796,20 +4799,20 @@
       </c>
     </row>
     <row r="66" spans="1:12">
-      <c r="A66" s="29" t="s">
+      <c r="A66" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="B66" s="29"/>
-      <c r="C66" s="29"/>
-      <c r="D66" s="29"/>
-      <c r="E66" s="29"/>
-      <c r="F66" s="29"/>
-      <c r="G66" s="29"/>
-      <c r="H66" s="29"/>
-      <c r="I66" s="29"/>
-      <c r="J66" s="29"/>
-      <c r="K66" s="29"/>
-      <c r="L66" s="29"/>
+      <c r="B66" s="35"/>
+      <c r="C66" s="35"/>
+      <c r="D66" s="35"/>
+      <c r="E66" s="35"/>
+      <c r="F66" s="35"/>
+      <c r="G66" s="35"/>
+      <c r="H66" s="35"/>
+      <c r="I66" s="35"/>
+      <c r="J66" s="35"/>
+      <c r="K66" s="35"/>
+      <c r="L66" s="35"/>
     </row>
     <row r="67" spans="1:12">
       <c r="A67" s="8">
@@ -5154,36 +5157,36 @@
       </c>
     </row>
     <row r="76" spans="1:12" ht="30" customHeight="1">
-      <c r="A76" s="33" t="s">
+      <c r="A76" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="B76" s="33"/>
-      <c r="C76" s="33"/>
-      <c r="D76" s="33"/>
-      <c r="E76" s="33"/>
-      <c r="F76" s="33"/>
-      <c r="G76" s="33"/>
-      <c r="H76" s="33"/>
-      <c r="I76" s="33"/>
-      <c r="J76" s="33"/>
-      <c r="K76" s="33"/>
-      <c r="L76" s="33"/>
+      <c r="B76" s="36"/>
+      <c r="C76" s="36"/>
+      <c r="D76" s="36"/>
+      <c r="E76" s="36"/>
+      <c r="F76" s="36"/>
+      <c r="G76" s="36"/>
+      <c r="H76" s="36"/>
+      <c r="I76" s="36"/>
+      <c r="J76" s="36"/>
+      <c r="K76" s="36"/>
+      <c r="L76" s="36"/>
     </row>
     <row r="77" spans="1:12">
-      <c r="A77" s="29" t="s">
+      <c r="A77" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="B77" s="29"/>
-      <c r="C77" s="29"/>
-      <c r="D77" s="29"/>
-      <c r="E77" s="29"/>
-      <c r="F77" s="29"/>
-      <c r="G77" s="29"/>
-      <c r="H77" s="29"/>
-      <c r="I77" s="29"/>
-      <c r="J77" s="29"/>
-      <c r="K77" s="29"/>
-      <c r="L77" s="29"/>
+      <c r="B77" s="35"/>
+      <c r="C77" s="35"/>
+      <c r="D77" s="35"/>
+      <c r="E77" s="35"/>
+      <c r="F77" s="35"/>
+      <c r="G77" s="35"/>
+      <c r="H77" s="35"/>
+      <c r="I77" s="35"/>
+      <c r="J77" s="35"/>
+      <c r="K77" s="35"/>
+      <c r="L77" s="35"/>
     </row>
     <row r="78" spans="1:12">
       <c r="A78" s="8">
@@ -5504,20 +5507,20 @@
       <c r="L86" s="8"/>
     </row>
     <row r="87" spans="1:12">
-      <c r="A87" s="29" t="s">
+      <c r="A87" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="B87" s="29"/>
-      <c r="C87" s="29"/>
-      <c r="D87" s="29"/>
-      <c r="E87" s="29"/>
-      <c r="F87" s="29"/>
-      <c r="G87" s="29"/>
-      <c r="H87" s="29"/>
-      <c r="I87" s="29"/>
-      <c r="J87" s="29"/>
-      <c r="K87" s="29"/>
-      <c r="L87" s="29"/>
+      <c r="B87" s="35"/>
+      <c r="C87" s="35"/>
+      <c r="D87" s="35"/>
+      <c r="E87" s="35"/>
+      <c r="F87" s="35"/>
+      <c r="G87" s="35"/>
+      <c r="H87" s="35"/>
+      <c r="I87" s="35"/>
+      <c r="J87" s="35"/>
+      <c r="K87" s="35"/>
+      <c r="L87" s="35"/>
     </row>
     <row r="88" spans="1:12">
       <c r="A88" s="8">
@@ -5814,20 +5817,20 @@
       <c r="L96" s="8"/>
     </row>
     <row r="97" spans="1:12">
-      <c r="A97" s="29" t="s">
+      <c r="A97" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="B97" s="29"/>
-      <c r="C97" s="29"/>
-      <c r="D97" s="29"/>
-      <c r="E97" s="29"/>
-      <c r="F97" s="29"/>
-      <c r="G97" s="29"/>
-      <c r="H97" s="29"/>
-      <c r="I97" s="29"/>
-      <c r="J97" s="29"/>
-      <c r="K97" s="29"/>
-      <c r="L97" s="29"/>
+      <c r="B97" s="35"/>
+      <c r="C97" s="35"/>
+      <c r="D97" s="35"/>
+      <c r="E97" s="35"/>
+      <c r="F97" s="35"/>
+      <c r="G97" s="35"/>
+      <c r="H97" s="35"/>
+      <c r="I97" s="35"/>
+      <c r="J97" s="35"/>
+      <c r="K97" s="35"/>
+      <c r="L97" s="35"/>
     </row>
     <row r="98" spans="1:12">
       <c r="A98" s="8">
@@ -6148,20 +6151,20 @@
       <c r="L106" s="8"/>
     </row>
     <row r="107" spans="1:12">
-      <c r="A107" s="29" t="s">
+      <c r="A107" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="B107" s="29"/>
-      <c r="C107" s="29"/>
-      <c r="D107" s="29"/>
-      <c r="E107" s="29"/>
-      <c r="F107" s="29"/>
-      <c r="G107" s="29"/>
-      <c r="H107" s="29"/>
-      <c r="I107" s="29"/>
-      <c r="J107" s="29"/>
-      <c r="K107" s="29"/>
-      <c r="L107" s="29"/>
+      <c r="B107" s="35"/>
+      <c r="C107" s="35"/>
+      <c r="D107" s="35"/>
+      <c r="E107" s="35"/>
+      <c r="F107" s="35"/>
+      <c r="G107" s="35"/>
+      <c r="H107" s="35"/>
+      <c r="I107" s="35"/>
+      <c r="J107" s="35"/>
+      <c r="K107" s="35"/>
+      <c r="L107" s="35"/>
     </row>
     <row r="108" spans="1:12">
       <c r="A108" s="8">
@@ -6458,20 +6461,20 @@
       <c r="L116" s="8"/>
     </row>
     <row r="117" spans="1:12">
-      <c r="A117" s="29" t="s">
+      <c r="A117" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="B117" s="29"/>
-      <c r="C117" s="29"/>
-      <c r="D117" s="29"/>
-      <c r="E117" s="29"/>
-      <c r="F117" s="29"/>
-      <c r="G117" s="29"/>
-      <c r="H117" s="29"/>
-      <c r="I117" s="29"/>
-      <c r="J117" s="29"/>
-      <c r="K117" s="29"/>
-      <c r="L117" s="29"/>
+      <c r="B117" s="35"/>
+      <c r="C117" s="35"/>
+      <c r="D117" s="35"/>
+      <c r="E117" s="35"/>
+      <c r="F117" s="35"/>
+      <c r="G117" s="35"/>
+      <c r="H117" s="35"/>
+      <c r="I117" s="35"/>
+      <c r="J117" s="35"/>
+      <c r="K117" s="35"/>
+      <c r="L117" s="35"/>
     </row>
     <row r="118" spans="1:12">
       <c r="A118" s="8">
@@ -6792,20 +6795,20 @@
       <c r="L126" s="3"/>
     </row>
     <row r="127" spans="1:12">
-      <c r="A127" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="B127" s="29"/>
-      <c r="C127" s="29"/>
-      <c r="D127" s="29"/>
-      <c r="E127" s="29"/>
-      <c r="F127" s="29"/>
-      <c r="G127" s="29"/>
-      <c r="H127" s="29"/>
-      <c r="I127" s="29"/>
-      <c r="J127" s="29"/>
-      <c r="K127" s="29"/>
-      <c r="L127" s="29"/>
+      <c r="A127" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="B127" s="35"/>
+      <c r="C127" s="35"/>
+      <c r="D127" s="35"/>
+      <c r="E127" s="35"/>
+      <c r="F127" s="35"/>
+      <c r="G127" s="35"/>
+      <c r="H127" s="35"/>
+      <c r="I127" s="35"/>
+      <c r="J127" s="35"/>
+      <c r="K127" s="35"/>
+      <c r="L127" s="35"/>
     </row>
     <row r="128" spans="1:12">
       <c r="A128" s="19">
@@ -6826,14 +6829,14 @@
       <c r="F128" s="19">
         <v>50</v>
       </c>
-      <c r="G128" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="H128" s="35"/>
-      <c r="I128" s="35"/>
-      <c r="J128" s="35"/>
-      <c r="K128" s="35"/>
-      <c r="L128" s="36"/>
+      <c r="G128" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="H128" s="38"/>
+      <c r="I128" s="38"/>
+      <c r="J128" s="38"/>
+      <c r="K128" s="38"/>
+      <c r="L128" s="39"/>
     </row>
     <row r="129" spans="1:12">
       <c r="A129" s="19">
@@ -6854,12 +6857,12 @@
       <c r="F129" s="19">
         <v>50</v>
       </c>
-      <c r="G129" s="37"/>
-      <c r="H129" s="38"/>
-      <c r="I129" s="38"/>
-      <c r="J129" s="38"/>
-      <c r="K129" s="38"/>
-      <c r="L129" s="39"/>
+      <c r="G129" s="40"/>
+      <c r="H129" s="41"/>
+      <c r="I129" s="41"/>
+      <c r="J129" s="41"/>
+      <c r="K129" s="41"/>
+      <c r="L129" s="42"/>
     </row>
     <row r="130" spans="1:12">
       <c r="A130" s="19">
@@ -6880,12 +6883,12 @@
       <c r="F130" s="19">
         <v>50</v>
       </c>
-      <c r="G130" s="37"/>
-      <c r="H130" s="38"/>
-      <c r="I130" s="38"/>
-      <c r="J130" s="38"/>
-      <c r="K130" s="38"/>
-      <c r="L130" s="39"/>
+      <c r="G130" s="40"/>
+      <c r="H130" s="41"/>
+      <c r="I130" s="41"/>
+      <c r="J130" s="41"/>
+      <c r="K130" s="41"/>
+      <c r="L130" s="42"/>
     </row>
     <row r="131" spans="1:12">
       <c r="A131" s="19">
@@ -6906,12 +6909,12 @@
       <c r="F131" s="19">
         <v>50</v>
       </c>
-      <c r="G131" s="37"/>
-      <c r="H131" s="38"/>
-      <c r="I131" s="38"/>
-      <c r="J131" s="38"/>
-      <c r="K131" s="38"/>
-      <c r="L131" s="39"/>
+      <c r="G131" s="40"/>
+      <c r="H131" s="41"/>
+      <c r="I131" s="41"/>
+      <c r="J131" s="41"/>
+      <c r="K131" s="41"/>
+      <c r="L131" s="42"/>
     </row>
     <row r="132" spans="1:12">
       <c r="A132" s="19">
@@ -6932,12 +6935,12 @@
       <c r="F132" s="19">
         <v>50</v>
       </c>
-      <c r="G132" s="37"/>
-      <c r="H132" s="38"/>
-      <c r="I132" s="38"/>
-      <c r="J132" s="38"/>
-      <c r="K132" s="38"/>
-      <c r="L132" s="39"/>
+      <c r="G132" s="40"/>
+      <c r="H132" s="41"/>
+      <c r="I132" s="41"/>
+      <c r="J132" s="41"/>
+      <c r="K132" s="41"/>
+      <c r="L132" s="42"/>
     </row>
     <row r="133" spans="1:12">
       <c r="A133" s="19">
@@ -6958,12 +6961,12 @@
       <c r="F133" s="19">
         <v>50</v>
       </c>
-      <c r="G133" s="37"/>
-      <c r="H133" s="38"/>
-      <c r="I133" s="38"/>
-      <c r="J133" s="38"/>
-      <c r="K133" s="38"/>
-      <c r="L133" s="39"/>
+      <c r="G133" s="40"/>
+      <c r="H133" s="41"/>
+      <c r="I133" s="41"/>
+      <c r="J133" s="41"/>
+      <c r="K133" s="41"/>
+      <c r="L133" s="42"/>
     </row>
     <row r="134" spans="1:12">
       <c r="A134" s="22">
@@ -6984,12 +6987,12 @@
       <c r="F134" s="19">
         <v>50</v>
       </c>
-      <c r="G134" s="37"/>
-      <c r="H134" s="38"/>
-      <c r="I134" s="38"/>
-      <c r="J134" s="38"/>
-      <c r="K134" s="38"/>
-      <c r="L134" s="39"/>
+      <c r="G134" s="40"/>
+      <c r="H134" s="41"/>
+      <c r="I134" s="41"/>
+      <c r="J134" s="41"/>
+      <c r="K134" s="41"/>
+      <c r="L134" s="42"/>
     </row>
     <row r="135" spans="1:12">
       <c r="A135" s="22">
@@ -7010,12 +7013,12 @@
       <c r="F135" s="19">
         <v>50</v>
       </c>
-      <c r="G135" s="37"/>
-      <c r="H135" s="38"/>
-      <c r="I135" s="38"/>
-      <c r="J135" s="38"/>
-      <c r="K135" s="38"/>
-      <c r="L135" s="39"/>
+      <c r="G135" s="40"/>
+      <c r="H135" s="41"/>
+      <c r="I135" s="41"/>
+      <c r="J135" s="41"/>
+      <c r="K135" s="41"/>
+      <c r="L135" s="42"/>
     </row>
     <row r="136" spans="1:12">
       <c r="A136" s="22">
@@ -7036,28 +7039,28 @@
       <c r="F136" s="19">
         <v>50</v>
       </c>
-      <c r="G136" s="40"/>
-      <c r="H136" s="41"/>
-      <c r="I136" s="41"/>
-      <c r="J136" s="41"/>
-      <c r="K136" s="41"/>
-      <c r="L136" s="42"/>
+      <c r="G136" s="43"/>
+      <c r="H136" s="44"/>
+      <c r="I136" s="44"/>
+      <c r="J136" s="44"/>
+      <c r="K136" s="44"/>
+      <c r="L136" s="45"/>
     </row>
     <row r="137" spans="1:12">
-      <c r="A137" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="B137" s="29"/>
-      <c r="C137" s="29"/>
-      <c r="D137" s="29"/>
-      <c r="E137" s="29"/>
-      <c r="F137" s="29"/>
-      <c r="G137" s="29"/>
-      <c r="H137" s="29"/>
-      <c r="I137" s="29"/>
-      <c r="J137" s="29"/>
-      <c r="K137" s="29"/>
-      <c r="L137" s="29"/>
+      <c r="A137" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="B137" s="35"/>
+      <c r="C137" s="35"/>
+      <c r="D137" s="35"/>
+      <c r="E137" s="35"/>
+      <c r="F137" s="35"/>
+      <c r="G137" s="35"/>
+      <c r="H137" s="35"/>
+      <c r="I137" s="35"/>
+      <c r="J137" s="35"/>
+      <c r="K137" s="35"/>
+      <c r="L137" s="35"/>
     </row>
     <row r="138" spans="1:12">
       <c r="A138" s="8">
@@ -7366,20 +7369,20 @@
       <c r="L146" s="3"/>
     </row>
     <row r="147" spans="1:12">
-      <c r="A147" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="B147" s="29"/>
-      <c r="C147" s="29"/>
-      <c r="D147" s="29"/>
-      <c r="E147" s="29"/>
-      <c r="F147" s="29"/>
-      <c r="G147" s="29"/>
-      <c r="H147" s="29"/>
-      <c r="I147" s="29"/>
-      <c r="J147" s="29"/>
-      <c r="K147" s="29"/>
-      <c r="L147" s="29"/>
+      <c r="A147" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B147" s="35"/>
+      <c r="C147" s="35"/>
+      <c r="D147" s="35"/>
+      <c r="E147" s="35"/>
+      <c r="F147" s="35"/>
+      <c r="G147" s="35"/>
+      <c r="H147" s="35"/>
+      <c r="I147" s="35"/>
+      <c r="J147" s="35"/>
+      <c r="K147" s="35"/>
+      <c r="L147" s="35"/>
     </row>
     <row r="148" spans="1:12">
       <c r="A148" s="8">
@@ -7687,17 +7690,319 @@
       <c r="K156" s="3"/>
       <c r="L156" s="3"/>
     </row>
+    <row r="157" spans="1:12">
+      <c r="A157" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="B157" s="35"/>
+      <c r="C157" s="35"/>
+      <c r="D157" s="35"/>
+      <c r="E157" s="35"/>
+      <c r="F157" s="35"/>
+      <c r="G157" s="35"/>
+      <c r="H157" s="35"/>
+      <c r="I157" s="35"/>
+      <c r="J157" s="35"/>
+      <c r="K157" s="35"/>
+      <c r="L157" s="35"/>
+    </row>
+    <row r="158" spans="1:12">
+      <c r="A158" s="8">
+        <v>10</v>
+      </c>
+      <c r="B158" s="9">
+        <v>4991</v>
+      </c>
+      <c r="C158" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D158" s="8">
+        <v>2500</v>
+      </c>
+      <c r="E158" s="8">
+        <v>10</v>
+      </c>
+      <c r="F158" s="8">
+        <v>50</v>
+      </c>
+      <c r="G158" s="3">
+        <v>4.99E-2</v>
+      </c>
+      <c r="H158" s="3">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="I158" s="3">
+        <v>2.9929999999999999</v>
+      </c>
+      <c r="J158" s="3">
+        <v>60135.23</v>
+      </c>
+      <c r="K158" s="3">
+        <v>5.987E-2</v>
+      </c>
+      <c r="L158" s="3">
+        <v>5.9520000000000003E-2</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12">
+      <c r="A159" s="8">
+        <v>50</v>
+      </c>
+      <c r="B159" s="9">
+        <v>22716</v>
+      </c>
+      <c r="C159" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D159" s="8">
+        <v>2500</v>
+      </c>
+      <c r="E159" s="8">
+        <v>10</v>
+      </c>
+      <c r="F159" s="8">
+        <v>50</v>
+      </c>
+      <c r="G159" s="3">
+        <v>6.0699999999999997E-2</v>
+      </c>
+      <c r="H159" s="3">
+        <v>9.7500000000000003E-2</v>
+      </c>
+      <c r="I159" s="3">
+        <v>3.4350000000000001</v>
+      </c>
+      <c r="J159" s="3">
+        <v>52400.99</v>
+      </c>
+      <c r="K159" s="3">
+        <v>6.8699999999999997E-2</v>
+      </c>
+      <c r="L159" s="3">
+        <v>6.837E-2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12">
+      <c r="A160" s="8">
+        <v>100</v>
+      </c>
+      <c r="B160" s="9">
+        <v>40333</v>
+      </c>
+      <c r="C160" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D160" s="8">
+        <v>2500</v>
+      </c>
+      <c r="E160" s="8">
+        <v>10</v>
+      </c>
+      <c r="F160" s="8">
+        <v>50</v>
+      </c>
+      <c r="G160" s="3">
+        <v>7.8899999999999998E-2</v>
+      </c>
+      <c r="H160" s="3">
+        <v>0.1143</v>
+      </c>
+      <c r="I160" s="3">
+        <v>4.4560000000000004</v>
+      </c>
+      <c r="J160" s="3">
+        <v>40396.82</v>
+      </c>
+      <c r="K160" s="3">
+        <v>8.9120000000000005E-2</v>
+      </c>
+      <c r="L160" s="3">
+        <v>8.881E-2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:12">
+      <c r="A161" s="8">
+        <v>250</v>
+      </c>
+      <c r="B161" s="9">
+        <v>98113</v>
+      </c>
+      <c r="C161" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D161" s="8">
+        <v>2500</v>
+      </c>
+      <c r="E161" s="8">
+        <v>10</v>
+      </c>
+      <c r="F161" s="8">
+        <v>50</v>
+      </c>
+      <c r="G161" s="3">
+        <v>0.2082</v>
+      </c>
+      <c r="H161" s="3">
+        <v>0.374</v>
+      </c>
+      <c r="I161" s="3">
+        <v>11.62</v>
+      </c>
+      <c r="J161" s="3">
+        <v>15490.05</v>
+      </c>
+      <c r="K161" s="3">
+        <v>0.23241000000000001</v>
+      </c>
+      <c r="L161" s="3">
+        <v>0.23047999999999999</v>
+      </c>
+    </row>
+    <row r="162" spans="1:12">
+      <c r="A162" s="8">
+        <v>500</v>
+      </c>
+      <c r="B162" s="9">
+        <v>191502</v>
+      </c>
+      <c r="C162" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D162" s="8">
+        <v>2500</v>
+      </c>
+      <c r="E162" s="8">
+        <v>10</v>
+      </c>
+      <c r="F162" s="8">
+        <v>50</v>
+      </c>
+      <c r="G162" s="3">
+        <v>0.65629999999999999</v>
+      </c>
+      <c r="H162" s="3">
+        <v>1.0221</v>
+      </c>
+      <c r="I162" s="3">
+        <v>35.658000000000001</v>
+      </c>
+      <c r="J162" s="3">
+        <v>5048.0200000000004</v>
+      </c>
+      <c r="K162" s="3">
+        <v>0.71314999999999995</v>
+      </c>
+      <c r="L162" s="3">
+        <v>0.70959000000000005</v>
+      </c>
+    </row>
+    <row r="163" spans="1:12">
+      <c r="A163" s="8">
+        <v>1000</v>
+      </c>
+      <c r="B163" s="9">
+        <v>375114</v>
+      </c>
+      <c r="C163" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D163" s="8">
+        <v>2500</v>
+      </c>
+      <c r="E163" s="8">
+        <v>10</v>
+      </c>
+      <c r="F163" s="8">
+        <v>50</v>
+      </c>
+      <c r="G163" s="3"/>
+      <c r="H163" s="3"/>
+      <c r="I163" s="3"/>
+      <c r="J163" s="3"/>
+      <c r="K163" s="3"/>
+      <c r="L163" s="3"/>
+    </row>
+    <row r="164" spans="1:12">
+      <c r="A164" s="5">
+        <v>1500</v>
+      </c>
+      <c r="B164" s="7">
+        <v>550078</v>
+      </c>
+      <c r="C164" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D164" s="5">
+        <v>2500</v>
+      </c>
+      <c r="E164" s="8">
+        <v>10</v>
+      </c>
+      <c r="F164" s="8">
+        <v>50</v>
+      </c>
+      <c r="G164" s="3"/>
+      <c r="H164" s="3"/>
+      <c r="I164" s="3"/>
+      <c r="J164" s="3"/>
+      <c r="K164" s="3"/>
+      <c r="L164" s="3"/>
+    </row>
+    <row r="165" spans="1:12">
+      <c r="A165" s="5">
+        <v>2000</v>
+      </c>
+      <c r="B165" s="7">
+        <v>725515</v>
+      </c>
+      <c r="C165" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D165" s="5">
+        <v>2500</v>
+      </c>
+      <c r="E165" s="8">
+        <v>10</v>
+      </c>
+      <c r="F165" s="8">
+        <v>50</v>
+      </c>
+      <c r="G165" s="3"/>
+      <c r="H165" s="3"/>
+      <c r="I165" s="3"/>
+      <c r="J165" s="3"/>
+      <c r="K165" s="3"/>
+      <c r="L165" s="3"/>
+    </row>
+    <row r="166" spans="1:12">
+      <c r="A166" s="5">
+        <v>2500</v>
+      </c>
+      <c r="B166" s="7">
+        <v>900517</v>
+      </c>
+      <c r="C166" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D166" s="5">
+        <v>2500</v>
+      </c>
+      <c r="E166" s="8">
+        <v>10</v>
+      </c>
+      <c r="F166" s="8">
+        <v>50</v>
+      </c>
+      <c r="G166" s="3"/>
+      <c r="H166" s="3"/>
+      <c r="I166" s="3"/>
+      <c r="J166" s="3"/>
+      <c r="K166" s="3"/>
+      <c r="L166" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="A31:L31"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A5:L5"/>
-    <mergeCell ref="A20:L20"/>
-    <mergeCell ref="A13:L13"/>
-    <mergeCell ref="A8:L8"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="G3:L3"/>
+  <mergeCells count="26">
+    <mergeCell ref="A157:L157"/>
     <mergeCell ref="A147:L147"/>
     <mergeCell ref="A24:L24"/>
     <mergeCell ref="A127:L127"/>
@@ -7714,6 +8019,15 @@
     <mergeCell ref="A56:L56"/>
     <mergeCell ref="A45:L45"/>
     <mergeCell ref="A36:L36"/>
+    <mergeCell ref="A31:L31"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="A20:L20"/>
+    <mergeCell ref="A13:L13"/>
+    <mergeCell ref="A8:L8"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="G3:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7744,11 +8058,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
       <c r="D1" s="24"/>
       <c r="E1" s="24"/>
     </row>
@@ -7759,28 +8073,28 @@
       <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:14" ht="15.75">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="54" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="55"/>
-      <c r="F3" s="52" t="s">
+      <c r="E3" s="56"/>
+      <c r="F3" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52" t="s">
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="52"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="6" t="s">
@@ -7827,22 +8141,22 @@
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="8">
@@ -8230,11 +8544,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
       <c r="D1" s="26"/>
       <c r="E1" s="26"/>
     </row>
@@ -8245,28 +8559,28 @@
       <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:14" ht="15.75">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="54" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="55"/>
-      <c r="F3" s="52" t="s">
+      <c r="E3" s="56"/>
+      <c r="F3" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52" t="s">
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="52"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="6" t="s">
@@ -8313,22 +8627,22 @@
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
+      <c r="A5" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="8">
@@ -8615,7 +8929,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
@@ -8636,11 +8950,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
       <c r="D1" s="25"/>
       <c r="E1" s="25"/>
     </row>
@@ -8651,28 +8965,28 @@
       <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:14" ht="15.75">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="54" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="55"/>
-      <c r="F3" s="52" t="s">
+      <c r="E3" s="56"/>
+      <c r="F3" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52" t="s">
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="52"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="6" t="s">
@@ -8719,22 +9033,22 @@
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="8">
@@ -9053,22 +9367,22 @@
       <c r="N14" s="3"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="29"/>
+      <c r="A15" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="35"/>
+      <c r="N15" s="35"/>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="8">
@@ -9140,7 +9454,7 @@
       <c r="K17" s="3">
         <v>8.1020000000000003</v>
       </c>
-      <c r="L17" s="56">
+      <c r="L17" s="29">
         <v>22215.73</v>
       </c>
       <c r="M17" s="3">

</xml_diff>